<commit_message>
update Product add and edit
</commit_message>
<xml_diff>
--- a/02.Design Document/Project Management.xlsx
+++ b/02.Design Document/Project Management.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/linnkoko/Desktop/Project/Food_Lab/Git/food_lab/02.Design Document/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E38CDF7-BE08-F942-A168-7C77DD648089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13E5994A-A087-1345-A53E-7A9FEDA2C8EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="500" windowWidth="37580" windowHeight="21100" activeTab="2" xr2:uid="{7BA0B221-245C-954E-96F6-3D960DADD312}"/>
+    <workbookView xWindow="640" yWindow="620" windowWidth="17960" windowHeight="20980" firstSheet="6" activeTab="10" xr2:uid="{7BA0B221-245C-954E-96F6-3D960DADD312}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="3" r:id="rId1"/>
@@ -28,7 +28,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="4">'Coin &amp; Order Flow'!$A$1:$U$57</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Cover!$A$1:$N$66</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="10">'DB Design'!$A$1:$P$292</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="10">'DB Design'!$A$1:$P$325</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="5">'Project Flow_Admin'!$A$1:$Q$291</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="6">'Project Flow_Customer'!$A$1:$T$305</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="7">'Project Flow_Kitchen'!$A$1:$U$95</definedName>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1118" uniqueCount="418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1183" uniqueCount="430">
   <si>
     <t>No</t>
   </si>
@@ -1321,6 +1321,42 @@
   <si>
     <t>Request,Cancel,Confirm,Reject,Working,Delivery,
 Complete</t>
+  </si>
+  <si>
+    <t>M_Product</t>
+  </si>
+  <si>
+    <t>product_name</t>
+  </si>
+  <si>
+    <t>product_type</t>
+  </si>
+  <si>
+    <t>product_taste</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>avaliable</t>
+  </si>
+  <si>
+    <t>0: avaliable , 1:not avaliable</t>
+  </si>
+  <si>
+    <t>M_Product_Detail</t>
+  </si>
+  <si>
+    <t>M_Product _ID</t>
+  </si>
+  <si>
+    <t>order</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>value</t>
   </si>
 </sst>
 </file>
@@ -2850,18 +2886,6 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2872,15 +2896,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="42" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="42" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="44" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2895,6 +2910,18 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2903,6 +2930,15 @@
     </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="42" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="42" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="44" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -20467,7 +20503,7 @@
       <c r="L64" s="261"/>
       <c r="M64" s="69">
         <f ca="1">NOW()</f>
-        <v>44573.893278587966</v>
+        <v>44573.955704398148</v>
       </c>
       <c r="N64" s="10"/>
     </row>
@@ -20612,7 +20648,7 @@
       </c>
       <c r="P2" s="280">
         <f ca="1">NOW()</f>
-        <v>44573.893278587966</v>
+        <v>44573.955704398148</v>
       </c>
       <c r="Q2" s="281"/>
     </row>
@@ -22057,10 +22093,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DA57DD3-54BE-0B47-9A75-C513CCBC9952}">
-  <dimension ref="A1:P292"/>
+  <dimension ref="A1:P317"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A120" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="J123" sqref="J123"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A286" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D313" sqref="D313:E313"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -22123,7 +22159,7 @@
       </c>
       <c r="O2" s="280">
         <f ca="1">NOW()</f>
-        <v>44573.893278587966</v>
+        <v>44573.955704398148</v>
       </c>
       <c r="P2" s="281"/>
     </row>
@@ -22461,10 +22497,10 @@
       <c r="C17" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="328" t="s">
+      <c r="D17" s="336" t="s">
         <v>30</v>
       </c>
-      <c r="E17" s="329"/>
+      <c r="E17" s="337"/>
       <c r="F17" s="25" t="s">
         <v>31</v>
       </c>
@@ -22483,12 +22519,12 @@
       <c r="K17" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="L17" s="330" t="s">
+      <c r="L17" s="338" t="s">
         <v>37</v>
       </c>
-      <c r="M17" s="330"/>
-      <c r="N17" s="330"/>
-      <c r="O17" s="331"/>
+      <c r="M17" s="338"/>
+      <c r="N17" s="338"/>
+      <c r="O17" s="339"/>
       <c r="P17" s="22"/>
     </row>
     <row r="18" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -22499,10 +22535,10 @@
       <c r="C18" s="27" t="s">
         <v>180</v>
       </c>
-      <c r="D18" s="332" t="s">
+      <c r="D18" s="328" t="s">
         <v>121</v>
       </c>
-      <c r="E18" s="333"/>
+      <c r="E18" s="329"/>
       <c r="F18" s="214"/>
       <c r="G18" s="214"/>
       <c r="H18" s="214" t="s">
@@ -22515,10 +22551,10 @@
         <v>128</v>
       </c>
       <c r="K18" s="214"/>
-      <c r="L18" s="334"/>
-      <c r="M18" s="334"/>
-      <c r="N18" s="334"/>
-      <c r="O18" s="335"/>
+      <c r="L18" s="330"/>
+      <c r="M18" s="330"/>
+      <c r="N18" s="330"/>
+      <c r="O18" s="331"/>
       <c r="P18" s="10"/>
     </row>
     <row r="19" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -22529,10 +22565,10 @@
       <c r="C19" s="27" t="s">
         <v>181</v>
       </c>
-      <c r="D19" s="332" t="s">
+      <c r="D19" s="328" t="s">
         <v>185</v>
       </c>
-      <c r="E19" s="333"/>
+      <c r="E19" s="329"/>
       <c r="F19" s="214"/>
       <c r="G19" s="214"/>
       <c r="H19" s="214" t="s">
@@ -22545,10 +22581,10 @@
         <v>128</v>
       </c>
       <c r="K19" s="214"/>
-      <c r="L19" s="334"/>
-      <c r="M19" s="334"/>
-      <c r="N19" s="334"/>
-      <c r="O19" s="335"/>
+      <c r="L19" s="330"/>
+      <c r="M19" s="330"/>
+      <c r="N19" s="330"/>
+      <c r="O19" s="331"/>
       <c r="P19" s="10"/>
     </row>
     <row r="20" spans="1:16" ht="59" customHeight="1" x14ac:dyDescent="0.2">
@@ -22559,10 +22595,10 @@
       <c r="C20" s="28" t="s">
         <v>182</v>
       </c>
-      <c r="D20" s="343" t="s">
+      <c r="D20" s="340" t="s">
         <v>186</v>
       </c>
-      <c r="E20" s="344"/>
+      <c r="E20" s="341"/>
       <c r="F20" s="214"/>
       <c r="G20" s="214"/>
       <c r="H20" s="214" t="s">
@@ -22575,12 +22611,12 @@
         <v>2</v>
       </c>
       <c r="K20" s="214"/>
-      <c r="L20" s="345" t="s">
+      <c r="L20" s="342" t="s">
         <v>205</v>
       </c>
-      <c r="M20" s="334"/>
-      <c r="N20" s="334"/>
-      <c r="O20" s="335"/>
+      <c r="M20" s="330"/>
+      <c r="N20" s="330"/>
+      <c r="O20" s="331"/>
       <c r="P20" s="10"/>
     </row>
     <row r="21" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -22591,10 +22627,10 @@
       <c r="C21" s="27" t="s">
         <v>183</v>
       </c>
-      <c r="D21" s="332" t="s">
+      <c r="D21" s="328" t="s">
         <v>187</v>
       </c>
-      <c r="E21" s="333"/>
+      <c r="E21" s="329"/>
       <c r="F21" s="214"/>
       <c r="G21" s="214"/>
       <c r="H21" s="214" t="s">
@@ -22605,12 +22641,12 @@
       </c>
       <c r="J21" s="214"/>
       <c r="K21" s="214"/>
-      <c r="L21" s="334" t="s">
+      <c r="L21" s="330" t="s">
         <v>189</v>
       </c>
-      <c r="M21" s="334"/>
-      <c r="N21" s="334"/>
-      <c r="O21" s="335"/>
+      <c r="M21" s="330"/>
+      <c r="N21" s="330"/>
+      <c r="O21" s="331"/>
       <c r="P21" s="10"/>
     </row>
     <row r="22" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -22621,10 +22657,10 @@
       <c r="C22" s="27" t="s">
         <v>184</v>
       </c>
-      <c r="D22" s="332" t="s">
+      <c r="D22" s="328" t="s">
         <v>193</v>
       </c>
-      <c r="E22" s="333"/>
+      <c r="E22" s="329"/>
       <c r="F22" s="214"/>
       <c r="G22" s="214"/>
       <c r="H22" s="214"/>
@@ -22633,28 +22669,28 @@
       </c>
       <c r="J22" s="214"/>
       <c r="K22" s="214"/>
-      <c r="L22" s="334"/>
-      <c r="M22" s="334"/>
-      <c r="N22" s="334"/>
-      <c r="O22" s="335"/>
+      <c r="L22" s="330"/>
+      <c r="M22" s="330"/>
+      <c r="N22" s="330"/>
+      <c r="O22" s="331"/>
       <c r="P22" s="10"/>
     </row>
     <row r="23" spans="1:16" ht="25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="9"/>
       <c r="B23" s="29"/>
       <c r="C23" s="30"/>
-      <c r="D23" s="339"/>
-      <c r="E23" s="340"/>
+      <c r="D23" s="332"/>
+      <c r="E23" s="333"/>
       <c r="F23" s="215"/>
       <c r="G23" s="215"/>
       <c r="H23" s="215"/>
       <c r="I23" s="31"/>
       <c r="J23" s="215"/>
       <c r="K23" s="215"/>
-      <c r="L23" s="341"/>
-      <c r="M23" s="341"/>
-      <c r="N23" s="341"/>
-      <c r="O23" s="342"/>
+      <c r="L23" s="334"/>
+      <c r="M23" s="334"/>
+      <c r="N23" s="334"/>
+      <c r="O23" s="335"/>
       <c r="P23" s="10"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
@@ -22759,10 +22795,10 @@
       <c r="C29" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="D29" s="328" t="s">
+      <c r="D29" s="336" t="s">
         <v>30</v>
       </c>
-      <c r="E29" s="329"/>
+      <c r="E29" s="337"/>
       <c r="F29" s="25" t="s">
         <v>31</v>
       </c>
@@ -22781,12 +22817,12 @@
       <c r="K29" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="L29" s="330" t="s">
+      <c r="L29" s="338" t="s">
         <v>37</v>
       </c>
-      <c r="M29" s="330"/>
-      <c r="N29" s="330"/>
-      <c r="O29" s="331"/>
+      <c r="M29" s="338"/>
+      <c r="N29" s="338"/>
+      <c r="O29" s="339"/>
       <c r="P29" s="10"/>
     </row>
     <row r="30" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -22797,10 +22833,10 @@
       <c r="C30" s="27" t="s">
         <v>206</v>
       </c>
-      <c r="D30" s="332" t="s">
+      <c r="D30" s="328" t="s">
         <v>208</v>
       </c>
-      <c r="E30" s="333"/>
+      <c r="E30" s="329"/>
       <c r="F30" s="214"/>
       <c r="G30" s="214"/>
       <c r="H30" s="214" t="s">
@@ -22811,12 +22847,12 @@
       </c>
       <c r="J30" s="214"/>
       <c r="K30" s="214"/>
-      <c r="L30" s="334" t="s">
+      <c r="L30" s="330" t="s">
         <v>210</v>
       </c>
-      <c r="M30" s="334"/>
-      <c r="N30" s="334"/>
-      <c r="O30" s="335"/>
+      <c r="M30" s="330"/>
+      <c r="N30" s="330"/>
+      <c r="O30" s="331"/>
       <c r="P30" s="10"/>
     </row>
     <row r="31" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -22827,10 +22863,10 @@
       <c r="C31" s="27" t="s">
         <v>207</v>
       </c>
-      <c r="D31" s="332" t="s">
+      <c r="D31" s="328" t="s">
         <v>209</v>
       </c>
-      <c r="E31" s="333"/>
+      <c r="E31" s="329"/>
       <c r="F31" s="214"/>
       <c r="G31" s="214"/>
       <c r="H31" s="214" t="s">
@@ -22841,10 +22877,10 @@
       </c>
       <c r="J31" s="214"/>
       <c r="K31" s="214"/>
-      <c r="L31" s="334"/>
-      <c r="M31" s="334"/>
-      <c r="N31" s="334"/>
-      <c r="O31" s="335"/>
+      <c r="L31" s="330"/>
+      <c r="M31" s="330"/>
+      <c r="N31" s="330"/>
+      <c r="O31" s="331"/>
       <c r="P31" s="10"/>
     </row>
     <row r="32" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -22859,10 +22895,10 @@
       <c r="I32" s="28"/>
       <c r="J32" s="214"/>
       <c r="K32" s="214"/>
-      <c r="L32" s="334"/>
-      <c r="M32" s="334"/>
-      <c r="N32" s="334"/>
-      <c r="O32" s="335"/>
+      <c r="L32" s="330"/>
+      <c r="M32" s="330"/>
+      <c r="N32" s="330"/>
+      <c r="O32" s="331"/>
       <c r="P32" s="10"/>
     </row>
     <row r="33" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -22877,10 +22913,10 @@
       <c r="I33" s="28"/>
       <c r="J33" s="214"/>
       <c r="K33" s="214"/>
-      <c r="L33" s="334"/>
-      <c r="M33" s="334"/>
-      <c r="N33" s="334"/>
-      <c r="O33" s="335"/>
+      <c r="L33" s="330"/>
+      <c r="M33" s="330"/>
+      <c r="N33" s="330"/>
+      <c r="O33" s="331"/>
       <c r="P33" s="10"/>
     </row>
     <row r="34" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -22895,28 +22931,28 @@
       <c r="I34" s="28"/>
       <c r="J34" s="214"/>
       <c r="K34" s="214"/>
-      <c r="L34" s="334"/>
-      <c r="M34" s="334"/>
-      <c r="N34" s="334"/>
-      <c r="O34" s="335"/>
+      <c r="L34" s="330"/>
+      <c r="M34" s="330"/>
+      <c r="N34" s="330"/>
+      <c r="O34" s="331"/>
       <c r="P34" s="10"/>
     </row>
     <row r="35" spans="1:16" ht="25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="9"/>
       <c r="B35" s="29"/>
       <c r="C35" s="30"/>
-      <c r="D35" s="339"/>
-      <c r="E35" s="340"/>
+      <c r="D35" s="332"/>
+      <c r="E35" s="333"/>
       <c r="F35" s="215"/>
       <c r="G35" s="215"/>
       <c r="H35" s="215"/>
       <c r="I35" s="31"/>
       <c r="J35" s="215"/>
       <c r="K35" s="215"/>
-      <c r="L35" s="341"/>
-      <c r="M35" s="341"/>
-      <c r="N35" s="341"/>
-      <c r="O35" s="342"/>
+      <c r="L35" s="334"/>
+      <c r="M35" s="334"/>
+      <c r="N35" s="334"/>
+      <c r="O35" s="335"/>
       <c r="P35" s="10"/>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.2">
@@ -23003,10 +23039,10 @@
       <c r="C40" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="D40" s="328" t="s">
+      <c r="D40" s="336" t="s">
         <v>30</v>
       </c>
-      <c r="E40" s="329"/>
+      <c r="E40" s="337"/>
       <c r="F40" s="25" t="s">
         <v>31</v>
       </c>
@@ -23025,12 +23061,12 @@
       <c r="K40" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="L40" s="330" t="s">
+      <c r="L40" s="338" t="s">
         <v>37</v>
       </c>
-      <c r="M40" s="330"/>
-      <c r="N40" s="330"/>
-      <c r="O40" s="331"/>
+      <c r="M40" s="338"/>
+      <c r="N40" s="338"/>
+      <c r="O40" s="339"/>
       <c r="P40" s="10"/>
     </row>
     <row r="41" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -23099,10 +23135,10 @@
       <c r="C43" s="27" t="s">
         <v>213</v>
       </c>
-      <c r="D43" s="332" t="s">
+      <c r="D43" s="328" t="s">
         <v>224</v>
       </c>
-      <c r="E43" s="333"/>
+      <c r="E43" s="329"/>
       <c r="F43" s="214"/>
       <c r="G43" s="214"/>
       <c r="H43" s="214" t="s">
@@ -23113,10 +23149,10 @@
       </c>
       <c r="J43" s="214"/>
       <c r="K43" s="214"/>
-      <c r="L43" s="334"/>
-      <c r="M43" s="334"/>
-      <c r="N43" s="334"/>
-      <c r="O43" s="335"/>
+      <c r="L43" s="330"/>
+      <c r="M43" s="330"/>
+      <c r="N43" s="330"/>
+      <c r="O43" s="331"/>
       <c r="P43" s="10"/>
     </row>
     <row r="44" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -23127,10 +23163,10 @@
       <c r="C44" s="27" t="s">
         <v>214</v>
       </c>
-      <c r="D44" s="332" t="s">
+      <c r="D44" s="328" t="s">
         <v>225</v>
       </c>
-      <c r="E44" s="333"/>
+      <c r="E44" s="329"/>
       <c r="F44" s="214"/>
       <c r="G44" s="214"/>
       <c r="H44" s="214" t="s">
@@ -23141,10 +23177,10 @@
       </c>
       <c r="J44" s="214"/>
       <c r="K44" s="214"/>
-      <c r="L44" s="334"/>
-      <c r="M44" s="334"/>
-      <c r="N44" s="334"/>
-      <c r="O44" s="335"/>
+      <c r="L44" s="330"/>
+      <c r="M44" s="330"/>
+      <c r="N44" s="330"/>
+      <c r="O44" s="331"/>
       <c r="P44" s="10"/>
     </row>
     <row r="45" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -23155,10 +23191,10 @@
       <c r="C45" s="27" t="s">
         <v>215</v>
       </c>
-      <c r="D45" s="332" t="s">
+      <c r="D45" s="328" t="s">
         <v>226</v>
       </c>
-      <c r="E45" s="333"/>
+      <c r="E45" s="329"/>
       <c r="F45" s="214"/>
       <c r="G45" s="214"/>
       <c r="H45" s="214" t="s">
@@ -23171,12 +23207,12 @@
       <c r="K45" s="254" t="s">
         <v>191</v>
       </c>
-      <c r="L45" s="334" t="s">
+      <c r="L45" s="330" t="s">
         <v>270</v>
       </c>
-      <c r="M45" s="334"/>
-      <c r="N45" s="334"/>
-      <c r="O45" s="335"/>
+      <c r="M45" s="330"/>
+      <c r="N45" s="330"/>
+      <c r="O45" s="331"/>
       <c r="P45" s="10"/>
     </row>
     <row r="46" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -23201,28 +23237,28 @@
       </c>
       <c r="J46" s="237"/>
       <c r="K46" s="237"/>
-      <c r="L46" s="334"/>
-      <c r="M46" s="334"/>
-      <c r="N46" s="334"/>
-      <c r="O46" s="335"/>
+      <c r="L46" s="330"/>
+      <c r="M46" s="330"/>
+      <c r="N46" s="330"/>
+      <c r="O46" s="331"/>
       <c r="P46" s="10"/>
     </row>
     <row r="47" spans="1:16" ht="25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="9"/>
       <c r="B47" s="29"/>
       <c r="C47" s="30"/>
-      <c r="D47" s="339"/>
-      <c r="E47" s="340"/>
+      <c r="D47" s="332"/>
+      <c r="E47" s="333"/>
       <c r="F47" s="215"/>
       <c r="G47" s="215"/>
       <c r="H47" s="215"/>
       <c r="I47" s="31"/>
       <c r="J47" s="215"/>
       <c r="K47" s="215"/>
-      <c r="L47" s="341"/>
-      <c r="M47" s="341"/>
-      <c r="N47" s="341"/>
-      <c r="O47" s="342"/>
+      <c r="L47" s="334"/>
+      <c r="M47" s="334"/>
+      <c r="N47" s="334"/>
+      <c r="O47" s="335"/>
       <c r="P47" s="10"/>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.2">
@@ -23309,10 +23345,10 @@
       <c r="C52" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="D52" s="328" t="s">
+      <c r="D52" s="336" t="s">
         <v>30</v>
       </c>
-      <c r="E52" s="329"/>
+      <c r="E52" s="337"/>
       <c r="F52" s="25" t="s">
         <v>31</v>
       </c>
@@ -23331,12 +23367,12 @@
       <c r="K52" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="L52" s="330" t="s">
+      <c r="L52" s="338" t="s">
         <v>37</v>
       </c>
-      <c r="M52" s="330"/>
-      <c r="N52" s="330"/>
-      <c r="O52" s="331"/>
+      <c r="M52" s="338"/>
+      <c r="N52" s="338"/>
+      <c r="O52" s="339"/>
       <c r="P52" s="10"/>
     </row>
     <row r="53" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -23347,10 +23383,10 @@
       <c r="C53" s="27" t="s">
         <v>217</v>
       </c>
-      <c r="D53" s="332" t="s">
+      <c r="D53" s="328" t="s">
         <v>218</v>
       </c>
-      <c r="E53" s="333"/>
+      <c r="E53" s="329"/>
       <c r="F53" s="214"/>
       <c r="G53" s="214"/>
       <c r="H53" s="214" t="s">
@@ -23363,12 +23399,12 @@
       <c r="K53" s="254" t="s">
         <v>191</v>
       </c>
-      <c r="L53" s="334" t="s">
+      <c r="L53" s="330" t="s">
         <v>329</v>
       </c>
-      <c r="M53" s="334"/>
-      <c r="N53" s="334"/>
-      <c r="O53" s="335"/>
+      <c r="M53" s="330"/>
+      <c r="N53" s="330"/>
+      <c r="O53" s="331"/>
       <c r="P53" s="10"/>
     </row>
     <row r="54" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -23493,10 +23529,10 @@
       <c r="C58" s="28" t="s">
         <v>219</v>
       </c>
-      <c r="D58" s="343" t="s">
+      <c r="D58" s="340" t="s">
         <v>227</v>
       </c>
-      <c r="E58" s="344"/>
+      <c r="E58" s="341"/>
       <c r="F58" s="214"/>
       <c r="G58" s="214"/>
       <c r="H58" s="214" t="s">
@@ -23507,12 +23543,12 @@
       </c>
       <c r="J58" s="214"/>
       <c r="K58" s="214"/>
-      <c r="L58" s="345" t="s">
+      <c r="L58" s="342" t="s">
         <v>409</v>
       </c>
-      <c r="M58" s="334"/>
-      <c r="N58" s="334"/>
-      <c r="O58" s="335"/>
+      <c r="M58" s="330"/>
+      <c r="N58" s="330"/>
+      <c r="O58" s="331"/>
       <c r="P58" s="10"/>
     </row>
     <row r="59" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -23523,10 +23559,10 @@
       <c r="C59" s="27" t="s">
         <v>220</v>
       </c>
-      <c r="D59" s="332" t="s">
+      <c r="D59" s="328" t="s">
         <v>228</v>
       </c>
-      <c r="E59" s="333"/>
+      <c r="E59" s="329"/>
       <c r="F59" s="214"/>
       <c r="G59" s="214"/>
       <c r="H59" s="214" t="s">
@@ -23537,10 +23573,10 @@
       </c>
       <c r="J59" s="214"/>
       <c r="K59" s="214"/>
-      <c r="L59" s="334"/>
-      <c r="M59" s="334"/>
-      <c r="N59" s="334"/>
-      <c r="O59" s="335"/>
+      <c r="L59" s="330"/>
+      <c r="M59" s="330"/>
+      <c r="N59" s="330"/>
+      <c r="O59" s="331"/>
       <c r="P59" s="10"/>
     </row>
     <row r="60" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -23551,10 +23587,10 @@
       <c r="C60" s="27" t="s">
         <v>221</v>
       </c>
-      <c r="D60" s="332" t="s">
+      <c r="D60" s="328" t="s">
         <v>229</v>
       </c>
-      <c r="E60" s="333"/>
+      <c r="E60" s="329"/>
       <c r="F60" s="214"/>
       <c r="G60" s="214"/>
       <c r="H60" s="214" t="s">
@@ -23567,30 +23603,30 @@
       <c r="K60" s="254" t="s">
         <v>191</v>
       </c>
-      <c r="L60" s="334" t="s">
+      <c r="L60" s="330" t="s">
         <v>270</v>
       </c>
-      <c r="M60" s="334"/>
-      <c r="N60" s="334"/>
-      <c r="O60" s="335"/>
+      <c r="M60" s="330"/>
+      <c r="N60" s="330"/>
+      <c r="O60" s="331"/>
       <c r="P60" s="10"/>
     </row>
     <row r="61" spans="1:16" ht="25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="9"/>
       <c r="B61" s="29"/>
       <c r="C61" s="30"/>
-      <c r="D61" s="339"/>
-      <c r="E61" s="340"/>
+      <c r="D61" s="332"/>
+      <c r="E61" s="333"/>
       <c r="F61" s="215"/>
       <c r="G61" s="215"/>
       <c r="H61" s="215"/>
       <c r="I61" s="31"/>
       <c r="J61" s="215"/>
       <c r="K61" s="215"/>
-      <c r="L61" s="341"/>
-      <c r="M61" s="341"/>
-      <c r="N61" s="341"/>
-      <c r="O61" s="342"/>
+      <c r="L61" s="334"/>
+      <c r="M61" s="334"/>
+      <c r="N61" s="334"/>
+      <c r="O61" s="335"/>
       <c r="P61" s="10"/>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.2">
@@ -23677,10 +23713,10 @@
       <c r="C66" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="D66" s="328" t="s">
+      <c r="D66" s="336" t="s">
         <v>30</v>
       </c>
-      <c r="E66" s="329"/>
+      <c r="E66" s="337"/>
       <c r="F66" s="25" t="s">
         <v>31</v>
       </c>
@@ -23699,12 +23735,12 @@
       <c r="K66" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="L66" s="330" t="s">
+      <c r="L66" s="338" t="s">
         <v>37</v>
       </c>
-      <c r="M66" s="330"/>
-      <c r="N66" s="330"/>
-      <c r="O66" s="331"/>
+      <c r="M66" s="338"/>
+      <c r="N66" s="338"/>
+      <c r="O66" s="339"/>
       <c r="P66" s="10"/>
     </row>
     <row r="67" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -23715,10 +23751,10 @@
       <c r="C67" s="27" t="s">
         <v>266</v>
       </c>
-      <c r="D67" s="332" t="s">
+      <c r="D67" s="328" t="s">
         <v>267</v>
       </c>
-      <c r="E67" s="333"/>
+      <c r="E67" s="329"/>
       <c r="F67" s="214"/>
       <c r="G67" s="214"/>
       <c r="H67" s="214" t="s">
@@ -23731,12 +23767,12 @@
       <c r="K67" s="254" t="s">
         <v>191</v>
       </c>
-      <c r="L67" s="334" t="s">
+      <c r="L67" s="330" t="s">
         <v>268</v>
       </c>
-      <c r="M67" s="334"/>
-      <c r="N67" s="334"/>
-      <c r="O67" s="335"/>
+      <c r="M67" s="330"/>
+      <c r="N67" s="330"/>
+      <c r="O67" s="331"/>
       <c r="P67" s="10"/>
     </row>
     <row r="68" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -23747,10 +23783,10 @@
       <c r="C68" s="27" t="s">
         <v>237</v>
       </c>
-      <c r="D68" s="332" t="s">
+      <c r="D68" s="328" t="s">
         <v>248</v>
       </c>
-      <c r="E68" s="333"/>
+      <c r="E68" s="329"/>
       <c r="F68" s="214"/>
       <c r="G68" s="214"/>
       <c r="H68" s="214" t="s">
@@ -23761,10 +23797,10 @@
       </c>
       <c r="J68" s="214"/>
       <c r="K68" s="214"/>
-      <c r="L68" s="334"/>
-      <c r="M68" s="334"/>
-      <c r="N68" s="334"/>
-      <c r="O68" s="335"/>
+      <c r="L68" s="330"/>
+      <c r="M68" s="330"/>
+      <c r="N68" s="330"/>
+      <c r="O68" s="331"/>
       <c r="P68" s="10"/>
     </row>
     <row r="69" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -23775,10 +23811,10 @@
       <c r="C69" s="27" t="s">
         <v>238</v>
       </c>
-      <c r="D69" s="332" t="s">
+      <c r="D69" s="328" t="s">
         <v>249</v>
       </c>
-      <c r="E69" s="333"/>
+      <c r="E69" s="329"/>
       <c r="F69" s="214"/>
       <c r="G69" s="214"/>
       <c r="H69" s="214" t="s">
@@ -23789,10 +23825,10 @@
       </c>
       <c r="J69" s="214"/>
       <c r="K69" s="214"/>
-      <c r="L69" s="334"/>
-      <c r="M69" s="334"/>
-      <c r="N69" s="334"/>
-      <c r="O69" s="335"/>
+      <c r="L69" s="330"/>
+      <c r="M69" s="330"/>
+      <c r="N69" s="330"/>
+      <c r="O69" s="331"/>
       <c r="P69" s="10"/>
     </row>
     <row r="70" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -23857,10 +23893,10 @@
       <c r="C72" s="28" t="s">
         <v>247</v>
       </c>
-      <c r="D72" s="332" t="s">
+      <c r="D72" s="328" t="s">
         <v>250</v>
       </c>
-      <c r="E72" s="333"/>
+      <c r="E72" s="329"/>
       <c r="F72" s="214"/>
       <c r="G72" s="214"/>
       <c r="H72" s="214"/>
@@ -23871,28 +23907,28 @@
         <v>255</v>
       </c>
       <c r="K72" s="214"/>
-      <c r="L72" s="345"/>
-      <c r="M72" s="334"/>
-      <c r="N72" s="334"/>
-      <c r="O72" s="335"/>
+      <c r="L72" s="342"/>
+      <c r="M72" s="330"/>
+      <c r="N72" s="330"/>
+      <c r="O72" s="331"/>
       <c r="P72" s="10"/>
     </row>
     <row r="73" spans="1:16" ht="25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A73" s="9"/>
       <c r="B73" s="29"/>
       <c r="C73" s="30"/>
-      <c r="D73" s="339"/>
-      <c r="E73" s="340"/>
+      <c r="D73" s="332"/>
+      <c r="E73" s="333"/>
       <c r="F73" s="215"/>
       <c r="G73" s="215"/>
       <c r="H73" s="215"/>
       <c r="I73" s="31"/>
       <c r="J73" s="215"/>
       <c r="K73" s="215"/>
-      <c r="L73" s="341"/>
-      <c r="M73" s="341"/>
-      <c r="N73" s="341"/>
-      <c r="O73" s="342"/>
+      <c r="L73" s="334"/>
+      <c r="M73" s="334"/>
+      <c r="N73" s="334"/>
+      <c r="O73" s="335"/>
       <c r="P73" s="10"/>
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.2">
@@ -23979,10 +24015,10 @@
       <c r="C78" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="D78" s="328" t="s">
+      <c r="D78" s="336" t="s">
         <v>30</v>
       </c>
-      <c r="E78" s="329"/>
+      <c r="E78" s="337"/>
       <c r="F78" s="25" t="s">
         <v>31</v>
       </c>
@@ -24001,12 +24037,12 @@
       <c r="K78" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="L78" s="330" t="s">
+      <c r="L78" s="338" t="s">
         <v>37</v>
       </c>
-      <c r="M78" s="330"/>
-      <c r="N78" s="330"/>
-      <c r="O78" s="331"/>
+      <c r="M78" s="338"/>
+      <c r="N78" s="338"/>
+      <c r="O78" s="339"/>
       <c r="P78" s="10"/>
     </row>
     <row r="79" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -24017,10 +24053,10 @@
       <c r="C79" s="27" t="s">
         <v>217</v>
       </c>
-      <c r="D79" s="332" t="s">
+      <c r="D79" s="328" t="s">
         <v>218</v>
       </c>
-      <c r="E79" s="333"/>
+      <c r="E79" s="329"/>
       <c r="F79" s="214"/>
       <c r="G79" s="214"/>
       <c r="H79" s="214" t="s">
@@ -24033,12 +24069,12 @@
       <c r="K79" s="254" t="s">
         <v>191</v>
       </c>
-      <c r="L79" s="334" t="s">
+      <c r="L79" s="330" t="s">
         <v>329</v>
       </c>
-      <c r="M79" s="334"/>
-      <c r="N79" s="334"/>
-      <c r="O79" s="335"/>
+      <c r="M79" s="330"/>
+      <c r="N79" s="330"/>
+      <c r="O79" s="331"/>
       <c r="P79" s="10"/>
     </row>
     <row r="80" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -24049,10 +24085,10 @@
       <c r="C80" s="27" t="s">
         <v>251</v>
       </c>
-      <c r="D80" s="332" t="s">
+      <c r="D80" s="328" t="s">
         <v>259</v>
       </c>
-      <c r="E80" s="333"/>
+      <c r="E80" s="329"/>
       <c r="F80" s="214"/>
       <c r="G80" s="214"/>
       <c r="H80" s="214" t="s">
@@ -24063,10 +24099,10 @@
       </c>
       <c r="J80" s="214"/>
       <c r="K80" s="214"/>
-      <c r="L80" s="334"/>
-      <c r="M80" s="334"/>
-      <c r="N80" s="334"/>
-      <c r="O80" s="335"/>
+      <c r="L80" s="330"/>
+      <c r="M80" s="330"/>
+      <c r="N80" s="330"/>
+      <c r="O80" s="331"/>
       <c r="P80" s="10"/>
     </row>
     <row r="81" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -24077,10 +24113,10 @@
       <c r="C81" s="27" t="s">
         <v>326</v>
       </c>
-      <c r="D81" s="332" t="s">
+      <c r="D81" s="328" t="s">
         <v>260</v>
       </c>
-      <c r="E81" s="333"/>
+      <c r="E81" s="329"/>
       <c r="F81" s="214"/>
       <c r="G81" s="214"/>
       <c r="H81" s="214" t="s">
@@ -24109,10 +24145,10 @@
       <c r="C82" s="27" t="s">
         <v>252</v>
       </c>
-      <c r="D82" s="332" t="s">
+      <c r="D82" s="328" t="s">
         <v>261</v>
       </c>
-      <c r="E82" s="333"/>
+      <c r="E82" s="329"/>
       <c r="F82" s="214"/>
       <c r="G82" s="214"/>
       <c r="H82" s="214" t="s">
@@ -24123,10 +24159,10 @@
       </c>
       <c r="J82" s="214"/>
       <c r="K82" s="241"/>
-      <c r="L82" s="334"/>
-      <c r="M82" s="334"/>
-      <c r="N82" s="334"/>
-      <c r="O82" s="335"/>
+      <c r="L82" s="330"/>
+      <c r="M82" s="330"/>
+      <c r="N82" s="330"/>
+      <c r="O82" s="331"/>
       <c r="P82" s="10"/>
     </row>
     <row r="83" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -24137,10 +24173,10 @@
       <c r="C83" s="27" t="s">
         <v>253</v>
       </c>
-      <c r="D83" s="332" t="s">
+      <c r="D83" s="328" t="s">
         <v>262</v>
       </c>
-      <c r="E83" s="333"/>
+      <c r="E83" s="329"/>
       <c r="F83" s="214"/>
       <c r="G83" s="214"/>
       <c r="H83" s="214" t="s">
@@ -24151,12 +24187,12 @@
       </c>
       <c r="J83" s="214"/>
       <c r="K83" s="241"/>
-      <c r="L83" s="334" t="s">
+      <c r="L83" s="330" t="s">
         <v>360</v>
       </c>
-      <c r="M83" s="334"/>
-      <c r="N83" s="334"/>
-      <c r="O83" s="335"/>
+      <c r="M83" s="330"/>
+      <c r="N83" s="330"/>
+      <c r="O83" s="331"/>
       <c r="P83" s="10"/>
     </row>
     <row r="84" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -24167,10 +24203,10 @@
       <c r="C84" s="27" t="s">
         <v>256</v>
       </c>
-      <c r="D84" s="332" t="s">
+      <c r="D84" s="328" t="s">
         <v>263</v>
       </c>
-      <c r="E84" s="333"/>
+      <c r="E84" s="329"/>
       <c r="F84" s="214"/>
       <c r="G84" s="214"/>
       <c r="H84" s="214" t="s">
@@ -24181,12 +24217,12 @@
       </c>
       <c r="J84" s="214"/>
       <c r="K84" s="241"/>
-      <c r="L84" s="334" t="s">
+      <c r="L84" s="330" t="s">
         <v>254</v>
       </c>
-      <c r="M84" s="334"/>
-      <c r="N84" s="334"/>
-      <c r="O84" s="335"/>
+      <c r="M84" s="330"/>
+      <c r="N84" s="330"/>
+      <c r="O84" s="331"/>
       <c r="P84" s="10"/>
     </row>
     <row r="85" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -24197,10 +24233,10 @@
       <c r="C85" s="28" t="s">
         <v>255</v>
       </c>
-      <c r="D85" s="332" t="s">
+      <c r="D85" s="328" t="s">
         <v>264</v>
       </c>
-      <c r="E85" s="333"/>
+      <c r="E85" s="329"/>
       <c r="F85" s="214"/>
       <c r="G85" s="214"/>
       <c r="H85" s="214" t="s">
@@ -24213,48 +24249,48 @@
       <c r="K85" s="254" t="s">
         <v>191</v>
       </c>
-      <c r="L85" s="336" t="s">
+      <c r="L85" s="343" t="s">
         <v>270</v>
       </c>
-      <c r="M85" s="337"/>
-      <c r="N85" s="337"/>
-      <c r="O85" s="338"/>
+      <c r="M85" s="344"/>
+      <c r="N85" s="344"/>
+      <c r="O85" s="345"/>
       <c r="P85" s="10"/>
     </row>
     <row r="86" spans="1:16" ht="24" x14ac:dyDescent="0.3">
       <c r="A86" s="9"/>
       <c r="B86" s="26"/>
       <c r="C86" s="27"/>
-      <c r="D86" s="332"/>
-      <c r="E86" s="333"/>
+      <c r="D86" s="328"/>
+      <c r="E86" s="329"/>
       <c r="F86" s="214"/>
       <c r="G86" s="214"/>
       <c r="H86" s="214"/>
       <c r="I86" s="28"/>
       <c r="J86" s="214"/>
       <c r="K86" s="214"/>
-      <c r="L86" s="334"/>
-      <c r="M86" s="334"/>
-      <c r="N86" s="334"/>
-      <c r="O86" s="335"/>
+      <c r="L86" s="330"/>
+      <c r="M86" s="330"/>
+      <c r="N86" s="330"/>
+      <c r="O86" s="331"/>
       <c r="P86" s="10"/>
     </row>
     <row r="87" spans="1:16" ht="25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A87" s="9"/>
       <c r="B87" s="29"/>
       <c r="C87" s="30"/>
-      <c r="D87" s="339"/>
-      <c r="E87" s="340"/>
+      <c r="D87" s="332"/>
+      <c r="E87" s="333"/>
       <c r="F87" s="215"/>
       <c r="G87" s="215"/>
       <c r="H87" s="215"/>
       <c r="I87" s="31"/>
       <c r="J87" s="215"/>
       <c r="K87" s="215"/>
-      <c r="L87" s="341"/>
-      <c r="M87" s="341"/>
-      <c r="N87" s="341"/>
-      <c r="O87" s="342"/>
+      <c r="L87" s="334"/>
+      <c r="M87" s="334"/>
+      <c r="N87" s="334"/>
+      <c r="O87" s="335"/>
       <c r="P87" s="10"/>
     </row>
     <row r="88" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -24341,10 +24377,10 @@
       <c r="C92" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="D92" s="328" t="s">
+      <c r="D92" s="336" t="s">
         <v>30</v>
       </c>
-      <c r="E92" s="329"/>
+      <c r="E92" s="337"/>
       <c r="F92" s="25" t="s">
         <v>31</v>
       </c>
@@ -24363,12 +24399,12 @@
       <c r="K92" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="L92" s="330" t="s">
+      <c r="L92" s="338" t="s">
         <v>37</v>
       </c>
-      <c r="M92" s="330"/>
-      <c r="N92" s="330"/>
-      <c r="O92" s="331"/>
+      <c r="M92" s="338"/>
+      <c r="N92" s="338"/>
+      <c r="O92" s="339"/>
       <c r="P92" s="10"/>
     </row>
     <row r="93" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -24379,10 +24415,10 @@
       <c r="C93" s="27" t="s">
         <v>322</v>
       </c>
-      <c r="D93" s="332" t="s">
+      <c r="D93" s="328" t="s">
         <v>269</v>
       </c>
-      <c r="E93" s="333"/>
+      <c r="E93" s="329"/>
       <c r="F93" s="214"/>
       <c r="G93" s="214"/>
       <c r="H93" s="214" t="s">
@@ -24395,12 +24431,12 @@
       <c r="K93" s="254" t="s">
         <v>191</v>
       </c>
-      <c r="L93" s="334" t="s">
+      <c r="L93" s="330" t="s">
         <v>265</v>
       </c>
-      <c r="M93" s="334"/>
-      <c r="N93" s="334"/>
-      <c r="O93" s="335"/>
+      <c r="M93" s="330"/>
+      <c r="N93" s="330"/>
+      <c r="O93" s="331"/>
       <c r="P93" s="10"/>
     </row>
     <row r="94" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -24411,10 +24447,10 @@
       <c r="C94" s="27" t="s">
         <v>255</v>
       </c>
-      <c r="D94" s="332" t="s">
+      <c r="D94" s="328" t="s">
         <v>264</v>
       </c>
-      <c r="E94" s="333"/>
+      <c r="E94" s="329"/>
       <c r="F94" s="214"/>
       <c r="G94" s="214"/>
       <c r="H94" s="214" t="s">
@@ -24427,12 +24463,12 @@
       <c r="K94" s="254" t="s">
         <v>191</v>
       </c>
-      <c r="L94" s="336" t="s">
+      <c r="L94" s="343" t="s">
         <v>270</v>
       </c>
-      <c r="M94" s="337"/>
-      <c r="N94" s="337"/>
-      <c r="O94" s="338"/>
+      <c r="M94" s="344"/>
+      <c r="N94" s="344"/>
+      <c r="O94" s="345"/>
       <c r="P94" s="10"/>
     </row>
     <row r="95" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -24443,10 +24479,10 @@
       <c r="C95" s="27" t="s">
         <v>257</v>
       </c>
-      <c r="D95" s="332" t="s">
+      <c r="D95" s="328" t="s">
         <v>271</v>
       </c>
-      <c r="E95" s="333"/>
+      <c r="E95" s="329"/>
       <c r="F95" s="214"/>
       <c r="G95" s="214"/>
       <c r="H95" s="214" t="s">
@@ -24471,10 +24507,10 @@
       <c r="C96" s="27" t="s">
         <v>258</v>
       </c>
-      <c r="D96" s="332" t="s">
+      <c r="D96" s="328" t="s">
         <v>272</v>
       </c>
-      <c r="E96" s="333"/>
+      <c r="E96" s="329"/>
       <c r="F96" s="214"/>
       <c r="G96" s="214"/>
       <c r="H96" s="214" t="s">
@@ -24485,10 +24521,10 @@
       </c>
       <c r="J96" s="214"/>
       <c r="K96" s="241"/>
-      <c r="L96" s="334"/>
-      <c r="M96" s="334"/>
-      <c r="N96" s="334"/>
-      <c r="O96" s="335"/>
+      <c r="L96" s="330"/>
+      <c r="M96" s="330"/>
+      <c r="N96" s="330"/>
+      <c r="O96" s="331"/>
       <c r="P96" s="10"/>
     </row>
     <row r="97" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -24499,10 +24535,10 @@
       <c r="C97" s="27" t="s">
         <v>247</v>
       </c>
-      <c r="D97" s="332" t="s">
+      <c r="D97" s="328" t="s">
         <v>311</v>
       </c>
-      <c r="E97" s="333"/>
+      <c r="E97" s="329"/>
       <c r="F97" s="214"/>
       <c r="G97" s="214"/>
       <c r="H97" s="214"/>
@@ -24513,10 +24549,10 @@
         <v>255</v>
       </c>
       <c r="K97" s="241"/>
-      <c r="L97" s="334"/>
-      <c r="M97" s="334"/>
-      <c r="N97" s="334"/>
-      <c r="O97" s="335"/>
+      <c r="L97" s="330"/>
+      <c r="M97" s="330"/>
+      <c r="N97" s="330"/>
+      <c r="O97" s="331"/>
       <c r="P97" s="10"/>
     </row>
     <row r="98" spans="1:16" ht="25" thickBot="1" x14ac:dyDescent="0.35">
@@ -24531,10 +24567,10 @@
       <c r="I98" s="31"/>
       <c r="J98" s="215"/>
       <c r="K98" s="215"/>
-      <c r="L98" s="341"/>
-      <c r="M98" s="341"/>
-      <c r="N98" s="341"/>
-      <c r="O98" s="342"/>
+      <c r="L98" s="334"/>
+      <c r="M98" s="334"/>
+      <c r="N98" s="334"/>
+      <c r="O98" s="335"/>
       <c r="P98" s="10"/>
     </row>
     <row r="99" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -24621,10 +24657,10 @@
       <c r="C103" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="D103" s="328" t="s">
+      <c r="D103" s="336" t="s">
         <v>30</v>
       </c>
-      <c r="E103" s="329"/>
+      <c r="E103" s="337"/>
       <c r="F103" s="25" t="s">
         <v>31</v>
       </c>
@@ -24643,12 +24679,12 @@
       <c r="K103" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="L103" s="330" t="s">
+      <c r="L103" s="338" t="s">
         <v>37</v>
       </c>
-      <c r="M103" s="330"/>
-      <c r="N103" s="330"/>
-      <c r="O103" s="331"/>
+      <c r="M103" s="338"/>
+      <c r="N103" s="338"/>
+      <c r="O103" s="339"/>
       <c r="P103" s="10"/>
     </row>
     <row r="104" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -24659,10 +24695,10 @@
       <c r="C104" s="27" t="s">
         <v>217</v>
       </c>
-      <c r="D104" s="332" t="s">
+      <c r="D104" s="328" t="s">
         <v>218</v>
       </c>
-      <c r="E104" s="333"/>
+      <c r="E104" s="329"/>
       <c r="F104" s="214"/>
       <c r="G104" s="214"/>
       <c r="H104" s="214" t="s">
@@ -24675,12 +24711,12 @@
       <c r="K104" s="254" t="s">
         <v>191</v>
       </c>
-      <c r="L104" s="334" t="s">
+      <c r="L104" s="330" t="s">
         <v>329</v>
       </c>
-      <c r="M104" s="334"/>
-      <c r="N104" s="334"/>
-      <c r="O104" s="335"/>
+      <c r="M104" s="330"/>
+      <c r="N104" s="330"/>
+      <c r="O104" s="331"/>
       <c r="P104" s="10"/>
     </row>
     <row r="105" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -24691,10 +24727,10 @@
       <c r="C105" s="27" t="s">
         <v>405</v>
       </c>
-      <c r="D105" s="332" t="s">
+      <c r="D105" s="328" t="s">
         <v>406</v>
       </c>
-      <c r="E105" s="333"/>
+      <c r="E105" s="329"/>
       <c r="F105" s="214"/>
       <c r="G105" s="214"/>
       <c r="H105" s="214" t="s">
@@ -24705,10 +24741,10 @@
       </c>
       <c r="J105" s="214"/>
       <c r="K105" s="214"/>
-      <c r="L105" s="334"/>
-      <c r="M105" s="334"/>
-      <c r="N105" s="334"/>
-      <c r="O105" s="335"/>
+      <c r="L105" s="330"/>
+      <c r="M105" s="330"/>
+      <c r="N105" s="330"/>
+      <c r="O105" s="331"/>
       <c r="P105" s="10"/>
     </row>
     <row r="106" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -24733,30 +24769,30 @@
       </c>
       <c r="J106" s="237"/>
       <c r="K106" s="237"/>
-      <c r="L106" s="336" t="s">
+      <c r="L106" s="343" t="s">
         <v>270</v>
       </c>
-      <c r="M106" s="337"/>
-      <c r="N106" s="337"/>
-      <c r="O106" s="338"/>
+      <c r="M106" s="344"/>
+      <c r="N106" s="344"/>
+      <c r="O106" s="345"/>
       <c r="P106" s="10"/>
     </row>
     <row r="107" spans="1:16" ht="25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A107" s="9"/>
       <c r="B107" s="29"/>
       <c r="C107" s="30"/>
-      <c r="D107" s="339"/>
-      <c r="E107" s="340"/>
+      <c r="D107" s="332"/>
+      <c r="E107" s="333"/>
       <c r="F107" s="215"/>
       <c r="G107" s="215"/>
       <c r="H107" s="215"/>
       <c r="I107" s="31"/>
       <c r="J107" s="215"/>
       <c r="K107" s="215"/>
-      <c r="L107" s="341"/>
-      <c r="M107" s="341"/>
-      <c r="N107" s="341"/>
-      <c r="O107" s="342"/>
+      <c r="L107" s="334"/>
+      <c r="M107" s="334"/>
+      <c r="N107" s="334"/>
+      <c r="O107" s="335"/>
       <c r="P107" s="10"/>
     </row>
     <row r="108" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -24843,10 +24879,10 @@
       <c r="C112" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="D112" s="328" t="s">
+      <c r="D112" s="336" t="s">
         <v>30</v>
       </c>
-      <c r="E112" s="329"/>
+      <c r="E112" s="337"/>
       <c r="F112" s="25" t="s">
         <v>31</v>
       </c>
@@ -24865,12 +24901,12 @@
       <c r="K112" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="L112" s="330" t="s">
+      <c r="L112" s="338" t="s">
         <v>37</v>
       </c>
-      <c r="M112" s="330"/>
-      <c r="N112" s="330"/>
-      <c r="O112" s="331"/>
+      <c r="M112" s="338"/>
+      <c r="N112" s="338"/>
+      <c r="O112" s="339"/>
       <c r="P112" s="10"/>
     </row>
     <row r="113" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -24881,10 +24917,10 @@
       <c r="C113" s="27" t="s">
         <v>322</v>
       </c>
-      <c r="D113" s="332" t="s">
+      <c r="D113" s="328" t="s">
         <v>269</v>
       </c>
-      <c r="E113" s="333"/>
+      <c r="E113" s="329"/>
       <c r="F113" s="214"/>
       <c r="G113" s="214"/>
       <c r="H113" s="214" t="s">
@@ -24897,12 +24933,12 @@
       <c r="K113" s="254" t="s">
         <v>191</v>
       </c>
-      <c r="L113" s="334" t="s">
+      <c r="L113" s="330" t="s">
         <v>265</v>
       </c>
-      <c r="M113" s="334"/>
-      <c r="N113" s="334"/>
-      <c r="O113" s="335"/>
+      <c r="M113" s="330"/>
+      <c r="N113" s="330"/>
+      <c r="O113" s="331"/>
       <c r="P113" s="10"/>
     </row>
     <row r="114" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -24913,10 +24949,10 @@
       <c r="C114" s="27" t="s">
         <v>330</v>
       </c>
-      <c r="D114" s="332" t="s">
+      <c r="D114" s="328" t="s">
         <v>245</v>
       </c>
-      <c r="E114" s="333"/>
+      <c r="E114" s="329"/>
       <c r="F114" s="214"/>
       <c r="G114" s="214"/>
       <c r="H114" s="214" t="s">
@@ -24927,12 +24963,12 @@
       </c>
       <c r="J114" s="214"/>
       <c r="K114" s="214"/>
-      <c r="L114" s="334" t="s">
+      <c r="L114" s="330" t="s">
         <v>346</v>
       </c>
-      <c r="M114" s="334"/>
-      <c r="N114" s="334"/>
-      <c r="O114" s="335"/>
+      <c r="M114" s="330"/>
+      <c r="N114" s="330"/>
+      <c r="O114" s="331"/>
       <c r="P114" s="10"/>
     </row>
     <row r="115" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -24967,18 +25003,18 @@
       <c r="A116" s="9"/>
       <c r="B116" s="29"/>
       <c r="C116" s="30"/>
-      <c r="D116" s="339"/>
-      <c r="E116" s="340"/>
+      <c r="D116" s="332"/>
+      <c r="E116" s="333"/>
       <c r="F116" s="215"/>
       <c r="G116" s="215"/>
       <c r="H116" s="215"/>
       <c r="I116" s="31"/>
       <c r="J116" s="215"/>
       <c r="K116" s="215"/>
-      <c r="L116" s="341"/>
-      <c r="M116" s="341"/>
-      <c r="N116" s="341"/>
-      <c r="O116" s="342"/>
+      <c r="L116" s="334"/>
+      <c r="M116" s="334"/>
+      <c r="N116" s="334"/>
+      <c r="O116" s="335"/>
       <c r="P116" s="10"/>
     </row>
     <row r="117" spans="1:16" ht="25" thickBot="1" x14ac:dyDescent="0.35">
@@ -25047,10 +25083,10 @@
       <c r="C120" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="D120" s="328" t="s">
+      <c r="D120" s="336" t="s">
         <v>30</v>
       </c>
-      <c r="E120" s="329"/>
+      <c r="E120" s="337"/>
       <c r="F120" s="25" t="s">
         <v>31</v>
       </c>
@@ -25069,12 +25105,12 @@
       <c r="K120" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="L120" s="330" t="s">
+      <c r="L120" s="338" t="s">
         <v>37</v>
       </c>
-      <c r="M120" s="330"/>
-      <c r="N120" s="330"/>
-      <c r="O120" s="331"/>
+      <c r="M120" s="338"/>
+      <c r="N120" s="338"/>
+      <c r="O120" s="339"/>
       <c r="P120" s="10"/>
     </row>
     <row r="121" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -25085,10 +25121,10 @@
       <c r="C121" s="27" t="s">
         <v>279</v>
       </c>
-      <c r="D121" s="332" t="s">
+      <c r="D121" s="328" t="s">
         <v>302</v>
       </c>
-      <c r="E121" s="333"/>
+      <c r="E121" s="329"/>
       <c r="F121" s="214" t="s">
         <v>191</v>
       </c>
@@ -25103,10 +25139,10 @@
         <v>128</v>
       </c>
       <c r="K121" s="214"/>
-      <c r="L121" s="336"/>
-      <c r="M121" s="337"/>
-      <c r="N121" s="337"/>
-      <c r="O121" s="338"/>
+      <c r="L121" s="343"/>
+      <c r="M121" s="344"/>
+      <c r="N121" s="344"/>
+      <c r="O121" s="345"/>
       <c r="P121" s="10"/>
     </row>
     <row r="122" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -25117,10 +25153,10 @@
       <c r="C122" s="27" t="s">
         <v>287</v>
       </c>
-      <c r="D122" s="332" t="s">
+      <c r="D122" s="328" t="s">
         <v>185</v>
       </c>
-      <c r="E122" s="333"/>
+      <c r="E122" s="329"/>
       <c r="F122" s="214"/>
       <c r="G122" s="214"/>
       <c r="H122" s="214" t="s">
@@ -25135,10 +25171,10 @@
       <c r="K122" s="214">
         <v>128</v>
       </c>
-      <c r="L122" s="334"/>
-      <c r="M122" s="334"/>
-      <c r="N122" s="334"/>
-      <c r="O122" s="335"/>
+      <c r="L122" s="330"/>
+      <c r="M122" s="330"/>
+      <c r="N122" s="330"/>
+      <c r="O122" s="331"/>
       <c r="P122" s="10"/>
     </row>
     <row r="123" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -25211,10 +25247,10 @@
       <c r="C125" s="27" t="s">
         <v>217</v>
       </c>
-      <c r="D125" s="332" t="s">
+      <c r="D125" s="328" t="s">
         <v>218</v>
       </c>
-      <c r="E125" s="333"/>
+      <c r="E125" s="329"/>
       <c r="F125" s="214"/>
       <c r="G125" s="214"/>
       <c r="H125" s="214" t="s">
@@ -25227,12 +25263,12 @@
       <c r="K125" s="254" t="s">
         <v>191</v>
       </c>
-      <c r="L125" s="334" t="s">
+      <c r="L125" s="330" t="s">
         <v>329</v>
       </c>
-      <c r="M125" s="334"/>
-      <c r="N125" s="334"/>
-      <c r="O125" s="335"/>
+      <c r="M125" s="330"/>
+      <c r="N125" s="330"/>
+      <c r="O125" s="331"/>
       <c r="P125" s="10"/>
     </row>
     <row r="126" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -25267,18 +25303,18 @@
       <c r="A127" s="9"/>
       <c r="B127" s="29"/>
       <c r="C127" s="30"/>
-      <c r="D127" s="339"/>
-      <c r="E127" s="340"/>
+      <c r="D127" s="332"/>
+      <c r="E127" s="333"/>
       <c r="F127" s="215"/>
       <c r="G127" s="215"/>
       <c r="H127" s="215"/>
       <c r="I127" s="31"/>
       <c r="J127" s="215"/>
       <c r="K127" s="215"/>
-      <c r="L127" s="341"/>
-      <c r="M127" s="341"/>
-      <c r="N127" s="341"/>
-      <c r="O127" s="342"/>
+      <c r="L127" s="334"/>
+      <c r="M127" s="334"/>
+      <c r="N127" s="334"/>
+      <c r="O127" s="335"/>
       <c r="P127" s="10"/>
     </row>
     <row r="128" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -25365,10 +25401,10 @@
       <c r="C132" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="D132" s="328" t="s">
+      <c r="D132" s="336" t="s">
         <v>30</v>
       </c>
-      <c r="E132" s="329"/>
+      <c r="E132" s="337"/>
       <c r="F132" s="25" t="s">
         <v>31</v>
       </c>
@@ -25387,12 +25423,12 @@
       <c r="K132" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="L132" s="330" t="s">
+      <c r="L132" s="338" t="s">
         <v>37</v>
       </c>
-      <c r="M132" s="330"/>
-      <c r="N132" s="330"/>
-      <c r="O132" s="331"/>
+      <c r="M132" s="338"/>
+      <c r="N132" s="338"/>
+      <c r="O132" s="339"/>
       <c r="P132" s="10"/>
     </row>
     <row r="133" spans="1:16" ht="257" customHeight="1" x14ac:dyDescent="0.2">
@@ -25403,10 +25439,10 @@
       <c r="C133" s="233" t="s">
         <v>291</v>
       </c>
-      <c r="D133" s="343" t="s">
+      <c r="D133" s="340" t="s">
         <v>299</v>
       </c>
-      <c r="E133" s="344"/>
+      <c r="E133" s="341"/>
       <c r="F133" s="214" t="s">
         <v>191</v>
       </c>
@@ -25437,10 +25473,10 @@
       <c r="C134" s="27" t="s">
         <v>298</v>
       </c>
-      <c r="D134" s="332" t="s">
+      <c r="D134" s="328" t="s">
         <v>300</v>
       </c>
-      <c r="E134" s="333"/>
+      <c r="E134" s="329"/>
       <c r="F134" s="214"/>
       <c r="G134" s="214"/>
       <c r="H134" s="214"/>
@@ -25465,10 +25501,10 @@
       <c r="C135" s="27" t="s">
         <v>278</v>
       </c>
-      <c r="D135" s="332" t="s">
+      <c r="D135" s="328" t="s">
         <v>301</v>
       </c>
-      <c r="E135" s="333"/>
+      <c r="E135" s="329"/>
       <c r="F135" s="214"/>
       <c r="G135" s="214"/>
       <c r="H135" s="214" t="s">
@@ -25495,10 +25531,10 @@
       <c r="C136" s="27" t="s">
         <v>280</v>
       </c>
-      <c r="D136" s="332" t="s">
+      <c r="D136" s="328" t="s">
         <v>303</v>
       </c>
-      <c r="E136" s="333"/>
+      <c r="E136" s="329"/>
       <c r="F136" s="214"/>
       <c r="G136" s="214"/>
       <c r="H136" s="214"/>
@@ -25521,10 +25557,10 @@
       <c r="C137" s="27" t="s">
         <v>281</v>
       </c>
-      <c r="D137" s="332" t="s">
+      <c r="D137" s="328" t="s">
         <v>304</v>
       </c>
-      <c r="E137" s="333"/>
+      <c r="E137" s="329"/>
       <c r="F137" s="214"/>
       <c r="G137" s="214"/>
       <c r="H137" s="214"/>
@@ -25549,10 +25585,10 @@
       <c r="C138" s="27" t="s">
         <v>282</v>
       </c>
-      <c r="D138" s="332" t="s">
+      <c r="D138" s="328" t="s">
         <v>304</v>
       </c>
-      <c r="E138" s="333"/>
+      <c r="E138" s="329"/>
       <c r="F138" s="214"/>
       <c r="G138" s="214"/>
       <c r="H138" s="214"/>
@@ -25577,10 +25613,10 @@
       <c r="C139" s="27" t="s">
         <v>283</v>
       </c>
-      <c r="D139" s="332" t="s">
+      <c r="D139" s="328" t="s">
         <v>304</v>
       </c>
-      <c r="E139" s="333"/>
+      <c r="E139" s="329"/>
       <c r="F139" s="214"/>
       <c r="G139" s="214"/>
       <c r="H139" s="214"/>
@@ -25605,10 +25641,10 @@
       <c r="C140" s="27" t="s">
         <v>284</v>
       </c>
-      <c r="D140" s="332" t="s">
+      <c r="D140" s="328" t="s">
         <v>305</v>
       </c>
-      <c r="E140" s="333"/>
+      <c r="E140" s="329"/>
       <c r="F140" s="214"/>
       <c r="G140" s="214"/>
       <c r="H140" s="214"/>
@@ -25635,10 +25671,10 @@
       <c r="C141" s="27" t="s">
         <v>285</v>
       </c>
-      <c r="D141" s="332" t="s">
+      <c r="D141" s="328" t="s">
         <v>306</v>
       </c>
-      <c r="E141" s="333"/>
+      <c r="E141" s="329"/>
       <c r="F141" s="214"/>
       <c r="G141" s="214"/>
       <c r="H141" s="214"/>
@@ -25691,10 +25727,10 @@
       <c r="C143" s="27" t="s">
         <v>286</v>
       </c>
-      <c r="D143" s="332" t="s">
+      <c r="D143" s="328" t="s">
         <v>307</v>
       </c>
-      <c r="E143" s="333"/>
+      <c r="E143" s="329"/>
       <c r="F143" s="214"/>
       <c r="G143" s="214"/>
       <c r="H143" s="214"/>
@@ -25719,10 +25755,10 @@
       <c r="C144" s="27" t="s">
         <v>288</v>
       </c>
-      <c r="D144" s="332" t="s">
+      <c r="D144" s="328" t="s">
         <v>309</v>
       </c>
-      <c r="E144" s="333"/>
+      <c r="E144" s="329"/>
       <c r="F144" s="214"/>
       <c r="G144" s="214"/>
       <c r="H144" s="214"/>
@@ -25747,10 +25783,10 @@
       <c r="C145" s="27" t="s">
         <v>289</v>
       </c>
-      <c r="D145" s="332" t="s">
+      <c r="D145" s="328" t="s">
         <v>308</v>
       </c>
-      <c r="E145" s="333"/>
+      <c r="E145" s="329"/>
       <c r="F145" s="214"/>
       <c r="G145" s="214"/>
       <c r="H145" s="214"/>
@@ -25775,10 +25811,10 @@
       <c r="C146" s="236" t="s">
         <v>290</v>
       </c>
-      <c r="D146" s="332" t="s">
+      <c r="D146" s="328" t="s">
         <v>310</v>
       </c>
-      <c r="E146" s="333"/>
+      <c r="E146" s="329"/>
       <c r="F146" s="237"/>
       <c r="G146" s="237"/>
       <c r="H146" s="237"/>
@@ -25799,8 +25835,8 @@
       <c r="A147" s="9"/>
       <c r="B147" s="29"/>
       <c r="C147" s="30"/>
-      <c r="D147" s="339"/>
-      <c r="E147" s="340"/>
+      <c r="D147" s="332"/>
+      <c r="E147" s="333"/>
       <c r="F147" s="215"/>
       <c r="G147" s="215"/>
       <c r="H147" s="215"/>
@@ -25915,10 +25951,10 @@
       <c r="C153" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="D153" s="328" t="s">
+      <c r="D153" s="336" t="s">
         <v>30</v>
       </c>
-      <c r="E153" s="329"/>
+      <c r="E153" s="337"/>
       <c r="F153" s="25" t="s">
         <v>31</v>
       </c>
@@ -25937,12 +25973,12 @@
       <c r="K153" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="L153" s="330" t="s">
+      <c r="L153" s="338" t="s">
         <v>37</v>
       </c>
-      <c r="M153" s="330"/>
-      <c r="N153" s="330"/>
-      <c r="O153" s="331"/>
+      <c r="M153" s="338"/>
+      <c r="N153" s="338"/>
+      <c r="O153" s="339"/>
       <c r="P153" s="10"/>
     </row>
     <row r="154" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -25953,10 +25989,10 @@
       <c r="C154" s="27" t="s">
         <v>312</v>
       </c>
-      <c r="D154" s="332" t="s">
+      <c r="D154" s="328" t="s">
         <v>315</v>
       </c>
-      <c r="E154" s="333"/>
+      <c r="E154" s="329"/>
       <c r="F154" s="214"/>
       <c r="G154" s="214"/>
       <c r="H154" s="214" t="s">
@@ -25969,10 +26005,10 @@
         <v>255</v>
       </c>
       <c r="K154" s="214"/>
-      <c r="L154" s="334"/>
-      <c r="M154" s="334"/>
-      <c r="N154" s="334"/>
-      <c r="O154" s="335"/>
+      <c r="L154" s="330"/>
+      <c r="M154" s="330"/>
+      <c r="N154" s="330"/>
+      <c r="O154" s="331"/>
       <c r="P154" s="10"/>
     </row>
     <row r="155" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -25983,10 +26019,10 @@
       <c r="C155" s="27" t="s">
         <v>313</v>
       </c>
-      <c r="D155" s="332" t="s">
+      <c r="D155" s="328" t="s">
         <v>316</v>
       </c>
-      <c r="E155" s="333"/>
+      <c r="E155" s="329"/>
       <c r="F155" s="214"/>
       <c r="G155" s="214"/>
       <c r="H155" s="214"/>
@@ -25997,10 +26033,10 @@
         <v>255</v>
       </c>
       <c r="K155" s="214"/>
-      <c r="L155" s="334"/>
-      <c r="M155" s="334"/>
-      <c r="N155" s="334"/>
-      <c r="O155" s="335"/>
+      <c r="L155" s="330"/>
+      <c r="M155" s="330"/>
+      <c r="N155" s="330"/>
+      <c r="O155" s="331"/>
       <c r="P155" s="10"/>
     </row>
     <row r="156" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -26025,10 +26061,10 @@
         <v>255</v>
       </c>
       <c r="K156" s="214"/>
-      <c r="L156" s="334"/>
-      <c r="M156" s="334"/>
-      <c r="N156" s="334"/>
-      <c r="O156" s="335"/>
+      <c r="L156" s="330"/>
+      <c r="M156" s="330"/>
+      <c r="N156" s="330"/>
+      <c r="O156" s="331"/>
       <c r="P156" s="10"/>
     </row>
     <row r="157" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -26039,10 +26075,10 @@
       <c r="C157" s="27" t="s">
         <v>314</v>
       </c>
-      <c r="D157" s="332" t="s">
+      <c r="D157" s="328" t="s">
         <v>317</v>
       </c>
-      <c r="E157" s="333"/>
+      <c r="E157" s="329"/>
       <c r="F157" s="214"/>
       <c r="G157" s="214"/>
       <c r="H157" s="214" t="s">
@@ -26053,12 +26089,12 @@
       </c>
       <c r="J157" s="214"/>
       <c r="K157" s="214"/>
-      <c r="L157" s="334" t="s">
+      <c r="L157" s="330" t="s">
         <v>347</v>
       </c>
-      <c r="M157" s="334"/>
-      <c r="N157" s="334"/>
-      <c r="O157" s="335"/>
+      <c r="M157" s="330"/>
+      <c r="N157" s="330"/>
+      <c r="O157" s="331"/>
       <c r="P157" s="10"/>
     </row>
     <row r="158" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -26069,10 +26105,10 @@
       <c r="C158" s="27" t="s">
         <v>318</v>
       </c>
-      <c r="D158" s="332" t="s">
+      <c r="D158" s="328" t="s">
         <v>319</v>
       </c>
-      <c r="E158" s="333"/>
+      <c r="E158" s="329"/>
       <c r="F158" s="214"/>
       <c r="G158" s="214"/>
       <c r="H158" s="214" t="s">
@@ -26085,30 +26121,30 @@
       <c r="K158" s="254" t="s">
         <v>191</v>
       </c>
-      <c r="L158" s="334" t="s">
+      <c r="L158" s="330" t="s">
         <v>270</v>
       </c>
-      <c r="M158" s="334"/>
-      <c r="N158" s="334"/>
-      <c r="O158" s="335"/>
+      <c r="M158" s="330"/>
+      <c r="N158" s="330"/>
+      <c r="O158" s="331"/>
       <c r="P158" s="10"/>
     </row>
     <row r="159" spans="1:16" ht="25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A159" s="9"/>
       <c r="B159" s="29"/>
       <c r="C159" s="30"/>
-      <c r="D159" s="339"/>
-      <c r="E159" s="340"/>
+      <c r="D159" s="332"/>
+      <c r="E159" s="333"/>
       <c r="F159" s="215"/>
       <c r="G159" s="215"/>
       <c r="H159" s="215"/>
       <c r="I159" s="31"/>
       <c r="J159" s="215"/>
       <c r="K159" s="215"/>
-      <c r="L159" s="341"/>
-      <c r="M159" s="341"/>
-      <c r="N159" s="341"/>
-      <c r="O159" s="342"/>
+      <c r="L159" s="334"/>
+      <c r="M159" s="334"/>
+      <c r="N159" s="334"/>
+      <c r="O159" s="335"/>
       <c r="P159" s="10"/>
     </row>
     <row r="160" spans="1:16" x14ac:dyDescent="0.2">
@@ -26195,10 +26231,10 @@
       <c r="C164" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="D164" s="328" t="s">
+      <c r="D164" s="336" t="s">
         <v>30</v>
       </c>
-      <c r="E164" s="329"/>
+      <c r="E164" s="337"/>
       <c r="F164" s="25" t="s">
         <v>31</v>
       </c>
@@ -26217,12 +26253,12 @@
       <c r="K164" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="L164" s="330" t="s">
+      <c r="L164" s="338" t="s">
         <v>37</v>
       </c>
-      <c r="M164" s="330"/>
-      <c r="N164" s="330"/>
-      <c r="O164" s="331"/>
+      <c r="M164" s="338"/>
+      <c r="N164" s="338"/>
+      <c r="O164" s="339"/>
       <c r="P164" s="10"/>
     </row>
     <row r="165" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -26233,10 +26269,10 @@
       <c r="C165" s="27" t="s">
         <v>312</v>
       </c>
-      <c r="D165" s="332" t="s">
+      <c r="D165" s="328" t="s">
         <v>320</v>
       </c>
-      <c r="E165" s="333"/>
+      <c r="E165" s="329"/>
       <c r="F165" s="214"/>
       <c r="G165" s="214"/>
       <c r="H165" s="214" t="s">
@@ -26249,10 +26285,10 @@
         <v>255</v>
       </c>
       <c r="K165" s="214"/>
-      <c r="L165" s="334"/>
-      <c r="M165" s="334"/>
-      <c r="N165" s="334"/>
-      <c r="O165" s="335"/>
+      <c r="L165" s="330"/>
+      <c r="M165" s="330"/>
+      <c r="N165" s="330"/>
+      <c r="O165" s="331"/>
       <c r="P165" s="10"/>
     </row>
     <row r="166" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -26263,10 +26299,10 @@
       <c r="C166" s="27" t="s">
         <v>313</v>
       </c>
-      <c r="D166" s="332" t="s">
+      <c r="D166" s="328" t="s">
         <v>321</v>
       </c>
-      <c r="E166" s="333"/>
+      <c r="E166" s="329"/>
       <c r="F166" s="214"/>
       <c r="G166" s="214"/>
       <c r="H166" s="214"/>
@@ -26277,10 +26313,10 @@
         <v>255</v>
       </c>
       <c r="K166" s="214"/>
-      <c r="L166" s="334"/>
-      <c r="M166" s="334"/>
-      <c r="N166" s="334"/>
-      <c r="O166" s="335"/>
+      <c r="L166" s="330"/>
+      <c r="M166" s="330"/>
+      <c r="N166" s="330"/>
+      <c r="O166" s="331"/>
       <c r="P166" s="10"/>
     </row>
     <row r="167" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -26305,30 +26341,30 @@
       <c r="K167" s="254" t="s">
         <v>191</v>
       </c>
-      <c r="L167" s="334" t="s">
+      <c r="L167" s="330" t="s">
         <v>323</v>
       </c>
-      <c r="M167" s="334"/>
-      <c r="N167" s="334"/>
-      <c r="O167" s="335"/>
+      <c r="M167" s="330"/>
+      <c r="N167" s="330"/>
+      <c r="O167" s="331"/>
       <c r="P167" s="10"/>
     </row>
     <row r="168" spans="1:16" ht="25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A168" s="9"/>
       <c r="B168" s="29"/>
       <c r="C168" s="30"/>
-      <c r="D168" s="339"/>
-      <c r="E168" s="340"/>
+      <c r="D168" s="332"/>
+      <c r="E168" s="333"/>
       <c r="F168" s="215"/>
       <c r="G168" s="215"/>
       <c r="H168" s="215"/>
       <c r="I168" s="31"/>
       <c r="J168" s="215"/>
       <c r="K168" s="215"/>
-      <c r="L168" s="341"/>
-      <c r="M168" s="341"/>
-      <c r="N168" s="341"/>
-      <c r="O168" s="342"/>
+      <c r="L168" s="334"/>
+      <c r="M168" s="334"/>
+      <c r="N168" s="334"/>
+      <c r="O168" s="335"/>
       <c r="P168" s="10"/>
     </row>
     <row r="169" spans="1:16" x14ac:dyDescent="0.2">
@@ -26415,10 +26451,10 @@
       <c r="C173" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="D173" s="328" t="s">
+      <c r="D173" s="336" t="s">
         <v>30</v>
       </c>
-      <c r="E173" s="329"/>
+      <c r="E173" s="337"/>
       <c r="F173" s="25" t="s">
         <v>31</v>
       </c>
@@ -26437,12 +26473,12 @@
       <c r="K173" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="L173" s="330" t="s">
+      <c r="L173" s="338" t="s">
         <v>37</v>
       </c>
-      <c r="M173" s="330"/>
-      <c r="N173" s="330"/>
-      <c r="O173" s="331"/>
+      <c r="M173" s="338"/>
+      <c r="N173" s="338"/>
+      <c r="O173" s="339"/>
       <c r="P173" s="10"/>
     </row>
     <row r="174" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -26453,10 +26489,10 @@
       <c r="C174" s="27" t="s">
         <v>312</v>
       </c>
-      <c r="D174" s="332" t="s">
+      <c r="D174" s="328" t="s">
         <v>320</v>
       </c>
-      <c r="E174" s="333"/>
+      <c r="E174" s="329"/>
       <c r="F174" s="214"/>
       <c r="G174" s="214"/>
       <c r="H174" s="214" t="s">
@@ -26469,10 +26505,10 @@
         <v>255</v>
       </c>
       <c r="K174" s="214"/>
-      <c r="L174" s="334"/>
-      <c r="M174" s="334"/>
-      <c r="N174" s="334"/>
-      <c r="O174" s="335"/>
+      <c r="L174" s="330"/>
+      <c r="M174" s="330"/>
+      <c r="N174" s="330"/>
+      <c r="O174" s="331"/>
       <c r="P174" s="10"/>
     </row>
     <row r="175" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -26483,10 +26519,10 @@
       <c r="C175" s="27" t="s">
         <v>313</v>
       </c>
-      <c r="D175" s="332" t="s">
+      <c r="D175" s="328" t="s">
         <v>321</v>
       </c>
-      <c r="E175" s="333"/>
+      <c r="E175" s="329"/>
       <c r="F175" s="214"/>
       <c r="G175" s="214"/>
       <c r="H175" s="214"/>
@@ -26497,10 +26533,10 @@
         <v>255</v>
       </c>
       <c r="K175" s="214"/>
-      <c r="L175" s="334"/>
-      <c r="M175" s="334"/>
-      <c r="N175" s="334"/>
-      <c r="O175" s="335"/>
+      <c r="L175" s="330"/>
+      <c r="M175" s="330"/>
+      <c r="N175" s="330"/>
+      <c r="O175" s="331"/>
       <c r="P175" s="10"/>
     </row>
     <row r="176" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -26525,30 +26561,30 @@
       <c r="K176" s="254" t="s">
         <v>191</v>
       </c>
-      <c r="L176" s="334" t="s">
+      <c r="L176" s="330" t="s">
         <v>268</v>
       </c>
-      <c r="M176" s="334"/>
-      <c r="N176" s="334"/>
-      <c r="O176" s="335"/>
+      <c r="M176" s="330"/>
+      <c r="N176" s="330"/>
+      <c r="O176" s="331"/>
       <c r="P176" s="10"/>
     </row>
     <row r="177" spans="1:16" ht="25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A177" s="9"/>
       <c r="B177" s="29"/>
       <c r="C177" s="30"/>
-      <c r="D177" s="339"/>
-      <c r="E177" s="340"/>
+      <c r="D177" s="332"/>
+      <c r="E177" s="333"/>
       <c r="F177" s="215"/>
       <c r="G177" s="215"/>
       <c r="H177" s="215"/>
       <c r="I177" s="31"/>
       <c r="J177" s="215"/>
       <c r="K177" s="215"/>
-      <c r="L177" s="341"/>
-      <c r="M177" s="341"/>
-      <c r="N177" s="341"/>
-      <c r="O177" s="342"/>
+      <c r="L177" s="334"/>
+      <c r="M177" s="334"/>
+      <c r="N177" s="334"/>
+      <c r="O177" s="335"/>
       <c r="P177" s="10"/>
     </row>
     <row r="178" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -26635,10 +26671,10 @@
       <c r="C182" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="D182" s="328" t="s">
+      <c r="D182" s="336" t="s">
         <v>30</v>
       </c>
-      <c r="E182" s="329"/>
+      <c r="E182" s="337"/>
       <c r="F182" s="25" t="s">
         <v>31</v>
       </c>
@@ -26657,12 +26693,12 @@
       <c r="K182" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="L182" s="330" t="s">
+      <c r="L182" s="338" t="s">
         <v>37</v>
       </c>
-      <c r="M182" s="330"/>
-      <c r="N182" s="330"/>
-      <c r="O182" s="331"/>
+      <c r="M182" s="338"/>
+      <c r="N182" s="338"/>
+      <c r="O182" s="339"/>
       <c r="P182" s="10"/>
     </row>
     <row r="183" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -26673,10 +26709,10 @@
       <c r="C183" s="27" t="s">
         <v>331</v>
       </c>
-      <c r="D183" s="332" t="s">
+      <c r="D183" s="328" t="s">
         <v>328</v>
       </c>
-      <c r="E183" s="333"/>
+      <c r="E183" s="329"/>
       <c r="F183" s="214"/>
       <c r="G183" s="214"/>
       <c r="H183" s="214" t="s">
@@ -26689,10 +26725,10 @@
         <v>255</v>
       </c>
       <c r="K183" s="214"/>
-      <c r="L183" s="334"/>
-      <c r="M183" s="334"/>
-      <c r="N183" s="334"/>
-      <c r="O183" s="335"/>
+      <c r="L183" s="330"/>
+      <c r="M183" s="330"/>
+      <c r="N183" s="330"/>
+      <c r="O183" s="331"/>
       <c r="P183" s="10"/>
     </row>
     <row r="184" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -26703,10 +26739,10 @@
       <c r="C184" s="27" t="s">
         <v>247</v>
       </c>
-      <c r="D184" s="332" t="s">
+      <c r="D184" s="328" t="s">
         <v>411</v>
       </c>
-      <c r="E184" s="333"/>
+      <c r="E184" s="329"/>
       <c r="F184" s="214"/>
       <c r="G184" s="214"/>
       <c r="H184" s="214"/>
@@ -26717,28 +26753,28 @@
         <v>255</v>
       </c>
       <c r="K184" s="214"/>
-      <c r="L184" s="334"/>
-      <c r="M184" s="334"/>
-      <c r="N184" s="334"/>
-      <c r="O184" s="335"/>
+      <c r="L184" s="330"/>
+      <c r="M184" s="330"/>
+      <c r="N184" s="330"/>
+      <c r="O184" s="331"/>
       <c r="P184" s="10"/>
     </row>
     <row r="185" spans="1:16" ht="25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A185" s="9"/>
       <c r="B185" s="29"/>
       <c r="C185" s="30"/>
-      <c r="D185" s="339"/>
-      <c r="E185" s="340"/>
+      <c r="D185" s="332"/>
+      <c r="E185" s="333"/>
       <c r="F185" s="215"/>
       <c r="G185" s="215"/>
       <c r="H185" s="215"/>
       <c r="I185" s="31"/>
       <c r="J185" s="215"/>
       <c r="K185" s="215"/>
-      <c r="L185" s="341"/>
-      <c r="M185" s="341"/>
-      <c r="N185" s="341"/>
-      <c r="O185" s="342"/>
+      <c r="L185" s="334"/>
+      <c r="M185" s="334"/>
+      <c r="N185" s="334"/>
+      <c r="O185" s="335"/>
       <c r="P185" s="10"/>
     </row>
     <row r="186" spans="1:16" x14ac:dyDescent="0.2">
@@ -26843,10 +26879,10 @@
       <c r="C191" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="D191" s="328" t="s">
+      <c r="D191" s="336" t="s">
         <v>30</v>
       </c>
-      <c r="E191" s="329"/>
+      <c r="E191" s="337"/>
       <c r="F191" s="25" t="s">
         <v>31</v>
       </c>
@@ -26865,12 +26901,12 @@
       <c r="K191" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="L191" s="330" t="s">
+      <c r="L191" s="338" t="s">
         <v>37</v>
       </c>
-      <c r="M191" s="330"/>
-      <c r="N191" s="330"/>
-      <c r="O191" s="331"/>
+      <c r="M191" s="338"/>
+      <c r="N191" s="338"/>
+      <c r="O191" s="339"/>
       <c r="P191" s="10"/>
     </row>
     <row r="192" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -26881,10 +26917,10 @@
       <c r="C192" s="27" t="s">
         <v>338</v>
       </c>
-      <c r="D192" s="332" t="s">
+      <c r="D192" s="328" t="s">
         <v>340</v>
       </c>
-      <c r="E192" s="333"/>
+      <c r="E192" s="329"/>
       <c r="F192" s="214"/>
       <c r="G192" s="214"/>
       <c r="H192" s="214" t="s">
@@ -26897,10 +26933,10 @@
         <v>255</v>
       </c>
       <c r="K192" s="214"/>
-      <c r="L192" s="334"/>
-      <c r="M192" s="334"/>
-      <c r="N192" s="334"/>
-      <c r="O192" s="335"/>
+      <c r="L192" s="330"/>
+      <c r="M192" s="330"/>
+      <c r="N192" s="330"/>
+      <c r="O192" s="331"/>
       <c r="P192" s="10"/>
     </row>
     <row r="193" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -26911,10 +26947,10 @@
       <c r="C193" s="27" t="s">
         <v>339</v>
       </c>
-      <c r="D193" s="332" t="s">
+      <c r="D193" s="328" t="s">
         <v>341</v>
       </c>
-      <c r="E193" s="333"/>
+      <c r="E193" s="329"/>
       <c r="F193" s="214"/>
       <c r="G193" s="214"/>
       <c r="H193" s="214" t="s">
@@ -26925,12 +26961,12 @@
       </c>
       <c r="J193" s="214"/>
       <c r="K193" s="214"/>
-      <c r="L193" s="334" t="s">
+      <c r="L193" s="330" t="s">
         <v>342</v>
       </c>
-      <c r="M193" s="334"/>
-      <c r="N193" s="334"/>
-      <c r="O193" s="335"/>
+      <c r="M193" s="330"/>
+      <c r="N193" s="330"/>
+      <c r="O193" s="331"/>
       <c r="P193" s="10"/>
     </row>
     <row r="194" spans="1:16" ht="25" thickBot="1" x14ac:dyDescent="0.35">
@@ -26955,10 +26991,10 @@
         <v>255</v>
       </c>
       <c r="K194" s="215"/>
-      <c r="L194" s="341"/>
-      <c r="M194" s="341"/>
-      <c r="N194" s="341"/>
-      <c r="O194" s="342"/>
+      <c r="L194" s="334"/>
+      <c r="M194" s="334"/>
+      <c r="N194" s="334"/>
+      <c r="O194" s="335"/>
       <c r="P194" s="10"/>
     </row>
     <row r="195" spans="1:16" x14ac:dyDescent="0.2">
@@ -27045,10 +27081,10 @@
       <c r="C199" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="D199" s="328" t="s">
+      <c r="D199" s="336" t="s">
         <v>30</v>
       </c>
-      <c r="E199" s="329"/>
+      <c r="E199" s="337"/>
       <c r="F199" s="25" t="s">
         <v>31</v>
       </c>
@@ -27067,12 +27103,12 @@
       <c r="K199" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="L199" s="330" t="s">
+      <c r="L199" s="338" t="s">
         <v>37</v>
       </c>
-      <c r="M199" s="330"/>
-      <c r="N199" s="330"/>
-      <c r="O199" s="331"/>
+      <c r="M199" s="338"/>
+      <c r="N199" s="338"/>
+      <c r="O199" s="339"/>
       <c r="P199" s="10"/>
     </row>
     <row r="200" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -27083,10 +27119,10 @@
       <c r="C200" s="27" t="s">
         <v>344</v>
       </c>
-      <c r="D200" s="332" t="s">
+      <c r="D200" s="328" t="s">
         <v>412</v>
       </c>
-      <c r="E200" s="333"/>
+      <c r="E200" s="329"/>
       <c r="F200" s="214"/>
       <c r="G200" s="214"/>
       <c r="H200" s="214" t="s">
@@ -27099,12 +27135,12 @@
         <v>255</v>
       </c>
       <c r="K200" s="214"/>
-      <c r="L200" s="334" t="s">
+      <c r="L200" s="330" t="s">
         <v>364</v>
       </c>
-      <c r="M200" s="334"/>
-      <c r="N200" s="334"/>
-      <c r="O200" s="335"/>
+      <c r="M200" s="330"/>
+      <c r="N200" s="330"/>
+      <c r="O200" s="331"/>
       <c r="P200" s="10"/>
     </row>
     <row r="201" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -27115,10 +27151,10 @@
       <c r="C201" s="27" t="s">
         <v>345</v>
       </c>
-      <c r="D201" s="332" t="s">
+      <c r="D201" s="328" t="s">
         <v>341</v>
       </c>
-      <c r="E201" s="333"/>
+      <c r="E201" s="329"/>
       <c r="F201" s="214"/>
       <c r="G201" s="214"/>
       <c r="H201" s="214" t="s">
@@ -27129,10 +27165,10 @@
       </c>
       <c r="J201" s="214"/>
       <c r="K201" s="214"/>
-      <c r="L201" s="334"/>
-      <c r="M201" s="334"/>
-      <c r="N201" s="334"/>
-      <c r="O201" s="335"/>
+      <c r="L201" s="330"/>
+      <c r="M201" s="330"/>
+      <c r="N201" s="330"/>
+      <c r="O201" s="331"/>
       <c r="P201" s="10"/>
     </row>
     <row r="202" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -27157,28 +27193,28 @@
         <v>255</v>
       </c>
       <c r="K202" s="237"/>
-      <c r="L202" s="334"/>
-      <c r="M202" s="334"/>
-      <c r="N202" s="334"/>
-      <c r="O202" s="335"/>
+      <c r="L202" s="330"/>
+      <c r="M202" s="330"/>
+      <c r="N202" s="330"/>
+      <c r="O202" s="331"/>
       <c r="P202" s="10"/>
     </row>
     <row r="203" spans="1:16" ht="25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A203" s="9"/>
       <c r="B203" s="29"/>
       <c r="C203" s="30"/>
-      <c r="D203" s="339"/>
-      <c r="E203" s="340"/>
+      <c r="D203" s="332"/>
+      <c r="E203" s="333"/>
       <c r="F203" s="215"/>
       <c r="G203" s="215"/>
       <c r="H203" s="215"/>
       <c r="I203" s="31"/>
       <c r="J203" s="215"/>
       <c r="K203" s="215"/>
-      <c r="L203" s="341"/>
-      <c r="M203" s="341"/>
-      <c r="N203" s="341"/>
-      <c r="O203" s="342"/>
+      <c r="L203" s="334"/>
+      <c r="M203" s="334"/>
+      <c r="N203" s="334"/>
+      <c r="O203" s="335"/>
       <c r="P203" s="10"/>
     </row>
     <row r="204" spans="1:16" x14ac:dyDescent="0.2">
@@ -27265,10 +27301,10 @@
       <c r="C208" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="D208" s="328" t="s">
+      <c r="D208" s="336" t="s">
         <v>30</v>
       </c>
-      <c r="E208" s="329"/>
+      <c r="E208" s="337"/>
       <c r="F208" s="25" t="s">
         <v>31</v>
       </c>
@@ -27287,12 +27323,12 @@
       <c r="K208" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="L208" s="330" t="s">
+      <c r="L208" s="338" t="s">
         <v>37</v>
       </c>
-      <c r="M208" s="330"/>
-      <c r="N208" s="330"/>
-      <c r="O208" s="331"/>
+      <c r="M208" s="338"/>
+      <c r="N208" s="338"/>
+      <c r="O208" s="339"/>
       <c r="P208" s="10"/>
     </row>
     <row r="209" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -27303,10 +27339,10 @@
       <c r="C209" s="27" t="s">
         <v>348</v>
       </c>
-      <c r="D209" s="332" t="s">
+      <c r="D209" s="328" t="s">
         <v>414</v>
       </c>
-      <c r="E209" s="333"/>
+      <c r="E209" s="329"/>
       <c r="F209" s="214"/>
       <c r="G209" s="214"/>
       <c r="H209" s="214" t="s">
@@ -27319,12 +27355,12 @@
         <v>255</v>
       </c>
       <c r="K209" s="214"/>
-      <c r="L209" s="334" t="s">
+      <c r="L209" s="330" t="s">
         <v>349</v>
       </c>
-      <c r="M209" s="334"/>
-      <c r="N209" s="334"/>
-      <c r="O209" s="335"/>
+      <c r="M209" s="330"/>
+      <c r="N209" s="330"/>
+      <c r="O209" s="331"/>
       <c r="P209" s="10"/>
     </row>
     <row r="210" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -27349,28 +27385,28 @@
         <v>255</v>
       </c>
       <c r="K210" s="237"/>
-      <c r="L210" s="334"/>
-      <c r="M210" s="334"/>
-      <c r="N210" s="334"/>
-      <c r="O210" s="335"/>
+      <c r="L210" s="330"/>
+      <c r="M210" s="330"/>
+      <c r="N210" s="330"/>
+      <c r="O210" s="331"/>
       <c r="P210" s="10"/>
     </row>
     <row r="211" spans="1:16" ht="25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A211" s="9"/>
       <c r="B211" s="29"/>
       <c r="C211" s="30"/>
-      <c r="D211" s="339"/>
-      <c r="E211" s="340"/>
+      <c r="D211" s="332"/>
+      <c r="E211" s="333"/>
       <c r="F211" s="215"/>
       <c r="G211" s="215"/>
       <c r="H211" s="215"/>
       <c r="I211" s="31"/>
       <c r="J211" s="215"/>
       <c r="K211" s="215"/>
-      <c r="L211" s="341"/>
-      <c r="M211" s="341"/>
-      <c r="N211" s="341"/>
-      <c r="O211" s="342"/>
+      <c r="L211" s="334"/>
+      <c r="M211" s="334"/>
+      <c r="N211" s="334"/>
+      <c r="O211" s="335"/>
       <c r="P211" s="10"/>
     </row>
     <row r="212" spans="1:16" x14ac:dyDescent="0.2">
@@ -27457,10 +27493,10 @@
       <c r="C216" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="D216" s="328" t="s">
+      <c r="D216" s="336" t="s">
         <v>30</v>
       </c>
-      <c r="E216" s="329"/>
+      <c r="E216" s="337"/>
       <c r="F216" s="25" t="s">
         <v>31</v>
       </c>
@@ -27479,12 +27515,12 @@
       <c r="K216" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="L216" s="330" t="s">
+      <c r="L216" s="338" t="s">
         <v>37</v>
       </c>
-      <c r="M216" s="330"/>
-      <c r="N216" s="330"/>
-      <c r="O216" s="331"/>
+      <c r="M216" s="338"/>
+      <c r="N216" s="338"/>
+      <c r="O216" s="339"/>
       <c r="P216" s="10"/>
     </row>
     <row r="217" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -27495,10 +27531,10 @@
       <c r="C217" s="27" t="s">
         <v>289</v>
       </c>
-      <c r="D217" s="332" t="s">
+      <c r="D217" s="328" t="s">
         <v>352</v>
       </c>
-      <c r="E217" s="333"/>
+      <c r="E217" s="329"/>
       <c r="F217" s="214"/>
       <c r="G217" s="214"/>
       <c r="H217" s="214" t="s">
@@ -27511,12 +27547,12 @@
         <v>255</v>
       </c>
       <c r="K217" s="214"/>
-      <c r="L217" s="334" t="s">
+      <c r="L217" s="330" t="s">
         <v>353</v>
       </c>
-      <c r="M217" s="334"/>
-      <c r="N217" s="334"/>
-      <c r="O217" s="335"/>
+      <c r="M217" s="330"/>
+      <c r="N217" s="330"/>
+      <c r="O217" s="331"/>
       <c r="P217" s="10"/>
     </row>
     <row r="218" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -27541,28 +27577,28 @@
         <v>255</v>
       </c>
       <c r="K218" s="237"/>
-      <c r="L218" s="334"/>
-      <c r="M218" s="334"/>
-      <c r="N218" s="334"/>
-      <c r="O218" s="335"/>
+      <c r="L218" s="330"/>
+      <c r="M218" s="330"/>
+      <c r="N218" s="330"/>
+      <c r="O218" s="331"/>
       <c r="P218" s="10"/>
     </row>
     <row r="219" spans="1:16" ht="25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A219" s="9"/>
       <c r="B219" s="29"/>
       <c r="C219" s="30"/>
-      <c r="D219" s="339"/>
-      <c r="E219" s="340"/>
+      <c r="D219" s="332"/>
+      <c r="E219" s="333"/>
       <c r="F219" s="215"/>
       <c r="G219" s="215"/>
       <c r="H219" s="215"/>
       <c r="I219" s="31"/>
       <c r="J219" s="215"/>
       <c r="K219" s="215"/>
-      <c r="L219" s="341"/>
-      <c r="M219" s="341"/>
-      <c r="N219" s="341"/>
-      <c r="O219" s="342"/>
+      <c r="L219" s="334"/>
+      <c r="M219" s="334"/>
+      <c r="N219" s="334"/>
+      <c r="O219" s="335"/>
       <c r="P219" s="10"/>
     </row>
     <row r="220" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -27649,10 +27685,10 @@
       <c r="C224" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="D224" s="328" t="s">
+      <c r="D224" s="336" t="s">
         <v>30</v>
       </c>
-      <c r="E224" s="329"/>
+      <c r="E224" s="337"/>
       <c r="F224" s="25" t="s">
         <v>31</v>
       </c>
@@ -27671,12 +27707,12 @@
       <c r="K224" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="L224" s="330" t="s">
+      <c r="L224" s="338" t="s">
         <v>37</v>
       </c>
-      <c r="M224" s="330"/>
-      <c r="N224" s="330"/>
-      <c r="O224" s="331"/>
+      <c r="M224" s="338"/>
+      <c r="N224" s="338"/>
+      <c r="O224" s="339"/>
       <c r="P224" s="10"/>
     </row>
     <row r="225" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -27687,10 +27723,10 @@
       <c r="C225" s="27" t="s">
         <v>383</v>
       </c>
-      <c r="D225" s="332" t="s">
+      <c r="D225" s="328" t="s">
         <v>390</v>
       </c>
-      <c r="E225" s="333"/>
+      <c r="E225" s="329"/>
       <c r="F225" s="214"/>
       <c r="G225" s="214"/>
       <c r="H225" s="214" t="s">
@@ -27703,12 +27739,12 @@
         <v>255</v>
       </c>
       <c r="K225" s="214"/>
-      <c r="L225" s="334" t="s">
+      <c r="L225" s="330" t="s">
         <v>391</v>
       </c>
-      <c r="M225" s="334"/>
-      <c r="N225" s="334"/>
-      <c r="O225" s="335"/>
+      <c r="M225" s="330"/>
+      <c r="N225" s="330"/>
+      <c r="O225" s="331"/>
       <c r="P225" s="10"/>
     </row>
     <row r="226" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -27733,28 +27769,28 @@
         <v>255</v>
       </c>
       <c r="K226" s="237"/>
-      <c r="L226" s="334"/>
-      <c r="M226" s="334"/>
-      <c r="N226" s="334"/>
-      <c r="O226" s="335"/>
+      <c r="L226" s="330"/>
+      <c r="M226" s="330"/>
+      <c r="N226" s="330"/>
+      <c r="O226" s="331"/>
       <c r="P226" s="10"/>
     </row>
     <row r="227" spans="1:16" ht="25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A227" s="9"/>
       <c r="B227" s="29"/>
       <c r="C227" s="30"/>
-      <c r="D227" s="339"/>
-      <c r="E227" s="340"/>
+      <c r="D227" s="332"/>
+      <c r="E227" s="333"/>
       <c r="F227" s="215"/>
       <c r="G227" s="215"/>
       <c r="H227" s="215"/>
       <c r="I227" s="31"/>
       <c r="J227" s="215"/>
       <c r="K227" s="215"/>
-      <c r="L227" s="341"/>
-      <c r="M227" s="341"/>
-      <c r="N227" s="341"/>
-      <c r="O227" s="342"/>
+      <c r="L227" s="334"/>
+      <c r="M227" s="334"/>
+      <c r="N227" s="334"/>
+      <c r="O227" s="335"/>
       <c r="P227" s="10"/>
     </row>
     <row r="228" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -27841,10 +27877,10 @@
       <c r="C232" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="D232" s="328" t="s">
+      <c r="D232" s="336" t="s">
         <v>30</v>
       </c>
-      <c r="E232" s="329"/>
+      <c r="E232" s="337"/>
       <c r="F232" s="25" t="s">
         <v>31</v>
       </c>
@@ -27863,12 +27899,12 @@
       <c r="K232" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="L232" s="330" t="s">
+      <c r="L232" s="338" t="s">
         <v>37</v>
       </c>
-      <c r="M232" s="330"/>
-      <c r="N232" s="330"/>
-      <c r="O232" s="331"/>
+      <c r="M232" s="338"/>
+      <c r="N232" s="338"/>
+      <c r="O232" s="339"/>
       <c r="P232" s="10"/>
     </row>
     <row r="233" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -27879,10 +27915,10 @@
       <c r="C233" s="27" t="s">
         <v>356</v>
       </c>
-      <c r="D233" s="332" t="s">
+      <c r="D233" s="328" t="s">
         <v>352</v>
       </c>
-      <c r="E233" s="333"/>
+      <c r="E233" s="329"/>
       <c r="F233" s="214"/>
       <c r="G233" s="214"/>
       <c r="H233" s="214" t="s">
@@ -27895,12 +27931,12 @@
         <v>255</v>
       </c>
       <c r="K233" s="214"/>
-      <c r="L233" s="334" t="s">
+      <c r="L233" s="330" t="s">
         <v>357</v>
       </c>
-      <c r="M233" s="334"/>
-      <c r="N233" s="334"/>
-      <c r="O233" s="335"/>
+      <c r="M233" s="330"/>
+      <c r="N233" s="330"/>
+      <c r="O233" s="331"/>
       <c r="P233" s="10"/>
     </row>
     <row r="234" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -27925,28 +27961,28 @@
         <v>255</v>
       </c>
       <c r="K234" s="237"/>
-      <c r="L234" s="345"/>
-      <c r="M234" s="334"/>
-      <c r="N234" s="334"/>
-      <c r="O234" s="335"/>
+      <c r="L234" s="342"/>
+      <c r="M234" s="330"/>
+      <c r="N234" s="330"/>
+      <c r="O234" s="331"/>
       <c r="P234" s="10"/>
     </row>
     <row r="235" spans="1:16" ht="25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A235" s="9"/>
       <c r="B235" s="29"/>
       <c r="C235" s="30"/>
-      <c r="D235" s="339"/>
-      <c r="E235" s="340"/>
+      <c r="D235" s="332"/>
+      <c r="E235" s="333"/>
       <c r="F235" s="215"/>
       <c r="G235" s="215"/>
       <c r="H235" s="215"/>
       <c r="I235" s="31"/>
       <c r="J235" s="215"/>
       <c r="K235" s="215"/>
-      <c r="L235" s="341"/>
-      <c r="M235" s="341"/>
-      <c r="N235" s="341"/>
-      <c r="O235" s="342"/>
+      <c r="L235" s="334"/>
+      <c r="M235" s="334"/>
+      <c r="N235" s="334"/>
+      <c r="O235" s="335"/>
       <c r="P235" s="10"/>
     </row>
     <row r="236" spans="1:16" x14ac:dyDescent="0.2">
@@ -28033,10 +28069,10 @@
       <c r="C240" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="D240" s="328" t="s">
+      <c r="D240" s="336" t="s">
         <v>30</v>
       </c>
-      <c r="E240" s="329"/>
+      <c r="E240" s="337"/>
       <c r="F240" s="25" t="s">
         <v>31</v>
       </c>
@@ -28055,12 +28091,12 @@
       <c r="K240" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="L240" s="330" t="s">
+      <c r="L240" s="338" t="s">
         <v>37</v>
       </c>
-      <c r="M240" s="330"/>
-      <c r="N240" s="330"/>
-      <c r="O240" s="331"/>
+      <c r="M240" s="338"/>
+      <c r="N240" s="338"/>
+      <c r="O240" s="339"/>
       <c r="P240" s="10"/>
     </row>
     <row r="241" spans="1:16" ht="56" customHeight="1" x14ac:dyDescent="0.2">
@@ -28071,10 +28107,10 @@
       <c r="C241" s="233" t="s">
         <v>359</v>
       </c>
-      <c r="D241" s="343" t="s">
+      <c r="D241" s="340" t="s">
         <v>227</v>
       </c>
-      <c r="E241" s="344"/>
+      <c r="E241" s="341"/>
       <c r="F241" s="214"/>
       <c r="G241" s="214"/>
       <c r="H241" s="214" t="s">
@@ -28087,12 +28123,12 @@
         <v>255</v>
       </c>
       <c r="K241" s="214"/>
-      <c r="L241" s="345" t="s">
+      <c r="L241" s="342" t="s">
         <v>417</v>
       </c>
-      <c r="M241" s="334"/>
-      <c r="N241" s="334"/>
-      <c r="O241" s="335"/>
+      <c r="M241" s="330"/>
+      <c r="N241" s="330"/>
+      <c r="O241" s="331"/>
       <c r="P241" s="10"/>
     </row>
     <row r="242" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -28117,28 +28153,28 @@
         <v>255</v>
       </c>
       <c r="K242" s="237"/>
-      <c r="L242" s="345"/>
-      <c r="M242" s="334"/>
-      <c r="N242" s="334"/>
-      <c r="O242" s="335"/>
+      <c r="L242" s="342"/>
+      <c r="M242" s="330"/>
+      <c r="N242" s="330"/>
+      <c r="O242" s="331"/>
       <c r="P242" s="10"/>
     </row>
     <row r="243" spans="1:16" ht="25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A243" s="9"/>
       <c r="B243" s="29"/>
       <c r="C243" s="30"/>
-      <c r="D243" s="339"/>
-      <c r="E243" s="340"/>
+      <c r="D243" s="332"/>
+      <c r="E243" s="333"/>
       <c r="F243" s="215"/>
       <c r="G243" s="215"/>
       <c r="H243" s="215"/>
       <c r="I243" s="31"/>
       <c r="J243" s="215"/>
       <c r="K243" s="215"/>
-      <c r="L243" s="341"/>
-      <c r="M243" s="341"/>
-      <c r="N243" s="341"/>
-      <c r="O243" s="342"/>
+      <c r="L243" s="334"/>
+      <c r="M243" s="334"/>
+      <c r="N243" s="334"/>
+      <c r="O243" s="335"/>
       <c r="P243" s="10"/>
     </row>
     <row r="244" spans="1:16" x14ac:dyDescent="0.2">
@@ -28225,10 +28261,10 @@
       <c r="C248" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="D248" s="328" t="s">
+      <c r="D248" s="336" t="s">
         <v>30</v>
       </c>
-      <c r="E248" s="329"/>
+      <c r="E248" s="337"/>
       <c r="F248" s="25" t="s">
         <v>31</v>
       </c>
@@ -28247,12 +28283,12 @@
       <c r="K248" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="L248" s="330" t="s">
+      <c r="L248" s="338" t="s">
         <v>37</v>
       </c>
-      <c r="M248" s="330"/>
-      <c r="N248" s="330"/>
-      <c r="O248" s="331"/>
+      <c r="M248" s="338"/>
+      <c r="N248" s="338"/>
+      <c r="O248" s="339"/>
       <c r="P248" s="10"/>
     </row>
     <row r="249" spans="1:16" ht="24" x14ac:dyDescent="0.2">
@@ -28263,10 +28299,10 @@
       <c r="C249" s="233" t="s">
         <v>359</v>
       </c>
-      <c r="D249" s="343" t="s">
+      <c r="D249" s="340" t="s">
         <v>362</v>
       </c>
-      <c r="E249" s="344"/>
+      <c r="E249" s="341"/>
       <c r="F249" s="214"/>
       <c r="G249" s="214"/>
       <c r="H249" s="214" t="s">
@@ -28279,12 +28315,12 @@
         <v>255</v>
       </c>
       <c r="K249" s="214"/>
-      <c r="L249" s="345" t="s">
+      <c r="L249" s="342" t="s">
         <v>363</v>
       </c>
-      <c r="M249" s="334"/>
-      <c r="N249" s="334"/>
-      <c r="O249" s="335"/>
+      <c r="M249" s="330"/>
+      <c r="N249" s="330"/>
+      <c r="O249" s="331"/>
       <c r="P249" s="10"/>
     </row>
     <row r="250" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -28309,28 +28345,28 @@
         <v>255</v>
       </c>
       <c r="K250" s="237"/>
-      <c r="L250" s="345"/>
-      <c r="M250" s="334"/>
-      <c r="N250" s="334"/>
-      <c r="O250" s="335"/>
+      <c r="L250" s="342"/>
+      <c r="M250" s="330"/>
+      <c r="N250" s="330"/>
+      <c r="O250" s="331"/>
       <c r="P250" s="10"/>
     </row>
     <row r="251" spans="1:16" ht="25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A251" s="9"/>
       <c r="B251" s="29"/>
       <c r="C251" s="30"/>
-      <c r="D251" s="339"/>
-      <c r="E251" s="340"/>
+      <c r="D251" s="332"/>
+      <c r="E251" s="333"/>
       <c r="F251" s="215"/>
       <c r="G251" s="215"/>
       <c r="H251" s="215"/>
       <c r="I251" s="31"/>
       <c r="J251" s="215"/>
       <c r="K251" s="215"/>
-      <c r="L251" s="341"/>
-      <c r="M251" s="341"/>
-      <c r="N251" s="341"/>
-      <c r="O251" s="342"/>
+      <c r="L251" s="334"/>
+      <c r="M251" s="334"/>
+      <c r="N251" s="334"/>
+      <c r="O251" s="335"/>
       <c r="P251" s="10"/>
     </row>
     <row r="252" spans="1:16" x14ac:dyDescent="0.2">
@@ -28419,10 +28455,10 @@
       <c r="C256" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="D256" s="328" t="s">
+      <c r="D256" s="336" t="s">
         <v>30</v>
       </c>
-      <c r="E256" s="329"/>
+      <c r="E256" s="337"/>
       <c r="F256" s="25" t="s">
         <v>31</v>
       </c>
@@ -28441,12 +28477,12 @@
       <c r="K256" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="L256" s="330" t="s">
+      <c r="L256" s="338" t="s">
         <v>37</v>
       </c>
-      <c r="M256" s="330"/>
-      <c r="N256" s="330"/>
-      <c r="O256" s="331"/>
+      <c r="M256" s="338"/>
+      <c r="N256" s="338"/>
+      <c r="O256" s="339"/>
       <c r="P256" s="10"/>
     </row>
     <row r="257" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -28457,10 +28493,10 @@
       <c r="C257" s="27" t="s">
         <v>266</v>
       </c>
-      <c r="D257" s="332" t="s">
+      <c r="D257" s="328" t="s">
         <v>267</v>
       </c>
-      <c r="E257" s="333"/>
+      <c r="E257" s="329"/>
       <c r="F257" s="214"/>
       <c r="G257" s="214"/>
       <c r="H257" s="214" t="s">
@@ -28475,12 +28511,12 @@
       <c r="K257" s="214" t="s">
         <v>191</v>
       </c>
-      <c r="L257" s="334" t="s">
+      <c r="L257" s="330" t="s">
         <v>268</v>
       </c>
-      <c r="M257" s="334"/>
-      <c r="N257" s="334"/>
-      <c r="O257" s="335"/>
+      <c r="M257" s="330"/>
+      <c r="N257" s="330"/>
+      <c r="O257" s="331"/>
       <c r="P257" s="10"/>
     </row>
     <row r="258" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -28491,10 +28527,10 @@
       <c r="C258" s="27" t="s">
         <v>377</v>
       </c>
-      <c r="D258" s="332" t="s">
+      <c r="D258" s="328" t="s">
         <v>378</v>
       </c>
-      <c r="E258" s="333"/>
+      <c r="E258" s="329"/>
       <c r="F258" s="214"/>
       <c r="G258" s="214"/>
       <c r="H258" s="214" t="s">
@@ -28507,10 +28543,10 @@
         <v>255</v>
       </c>
       <c r="K258" s="214"/>
-      <c r="L258" s="334"/>
-      <c r="M258" s="334"/>
-      <c r="N258" s="334"/>
-      <c r="O258" s="335"/>
+      <c r="L258" s="330"/>
+      <c r="M258" s="330"/>
+      <c r="N258" s="330"/>
+      <c r="O258" s="331"/>
       <c r="P258" s="10"/>
     </row>
     <row r="259" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -28521,10 +28557,10 @@
       <c r="C259" s="27" t="s">
         <v>376</v>
       </c>
-      <c r="D259" s="332" t="s">
+      <c r="D259" s="328" t="s">
         <v>379</v>
       </c>
-      <c r="E259" s="333"/>
+      <c r="E259" s="329"/>
       <c r="F259" s="214"/>
       <c r="G259" s="214"/>
       <c r="H259" s="214"/>
@@ -28535,28 +28571,28 @@
         <v>255</v>
       </c>
       <c r="K259" s="214"/>
-      <c r="L259" s="334"/>
-      <c r="M259" s="334"/>
-      <c r="N259" s="334"/>
-      <c r="O259" s="335"/>
+      <c r="L259" s="330"/>
+      <c r="M259" s="330"/>
+      <c r="N259" s="330"/>
+      <c r="O259" s="331"/>
       <c r="P259" s="10"/>
     </row>
     <row r="260" spans="1:16" ht="25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A260" s="9"/>
       <c r="B260" s="29"/>
       <c r="C260" s="30"/>
-      <c r="D260" s="339"/>
-      <c r="E260" s="340"/>
+      <c r="D260" s="332"/>
+      <c r="E260" s="333"/>
       <c r="F260" s="215"/>
       <c r="G260" s="215"/>
       <c r="H260" s="215"/>
       <c r="I260" s="31"/>
       <c r="J260" s="215"/>
       <c r="K260" s="215"/>
-      <c r="L260" s="341"/>
-      <c r="M260" s="341"/>
-      <c r="N260" s="341"/>
-      <c r="O260" s="342"/>
+      <c r="L260" s="334"/>
+      <c r="M260" s="334"/>
+      <c r="N260" s="334"/>
+      <c r="O260" s="335"/>
       <c r="P260" s="10"/>
     </row>
     <row r="261" spans="1:16" x14ac:dyDescent="0.2">
@@ -28645,10 +28681,10 @@
       <c r="C265" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="D265" s="328" t="s">
+      <c r="D265" s="336" t="s">
         <v>30</v>
       </c>
-      <c r="E265" s="329"/>
+      <c r="E265" s="337"/>
       <c r="F265" s="25" t="s">
         <v>31</v>
       </c>
@@ -28667,12 +28703,12 @@
       <c r="K265" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="L265" s="330" t="s">
+      <c r="L265" s="338" t="s">
         <v>37</v>
       </c>
-      <c r="M265" s="330"/>
-      <c r="N265" s="330"/>
-      <c r="O265" s="331"/>
+      <c r="M265" s="338"/>
+      <c r="N265" s="338"/>
+      <c r="O265" s="339"/>
       <c r="P265" s="10"/>
     </row>
     <row r="266" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -28683,10 +28719,10 @@
       <c r="C266" s="27" t="s">
         <v>380</v>
       </c>
-      <c r="D266" s="332" t="s">
+      <c r="D266" s="328" t="s">
         <v>381</v>
       </c>
-      <c r="E266" s="333"/>
+      <c r="E266" s="329"/>
       <c r="F266" s="214"/>
       <c r="G266" s="214"/>
       <c r="H266" s="214" t="s">
@@ -28699,10 +28735,10 @@
         <v>255</v>
       </c>
       <c r="K266" s="214"/>
-      <c r="L266" s="334"/>
-      <c r="M266" s="334"/>
-      <c r="N266" s="334"/>
-      <c r="O266" s="335"/>
+      <c r="L266" s="330"/>
+      <c r="M266" s="330"/>
+      <c r="N266" s="330"/>
+      <c r="O266" s="331"/>
       <c r="P266" s="10"/>
     </row>
     <row r="267" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -28713,10 +28749,10 @@
       <c r="C267" s="27" t="s">
         <v>376</v>
       </c>
-      <c r="D267" s="332" t="s">
+      <c r="D267" s="328" t="s">
         <v>382</v>
       </c>
-      <c r="E267" s="333"/>
+      <c r="E267" s="329"/>
       <c r="F267" s="214"/>
       <c r="G267" s="214"/>
       <c r="H267" s="214"/>
@@ -28727,10 +28763,10 @@
         <v>255</v>
       </c>
       <c r="K267" s="214"/>
-      <c r="L267" s="334"/>
-      <c r="M267" s="334"/>
-      <c r="N267" s="334"/>
-      <c r="O267" s="335"/>
+      <c r="L267" s="330"/>
+      <c r="M267" s="330"/>
+      <c r="N267" s="330"/>
+      <c r="O267" s="331"/>
       <c r="P267" s="10"/>
     </row>
     <row r="268" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -28753,30 +28789,30 @@
       </c>
       <c r="J268" s="214"/>
       <c r="K268" s="214"/>
-      <c r="L268" s="334" t="s">
+      <c r="L268" s="330" t="s">
         <v>416</v>
       </c>
-      <c r="M268" s="334"/>
-      <c r="N268" s="334"/>
-      <c r="O268" s="335"/>
+      <c r="M268" s="330"/>
+      <c r="N268" s="330"/>
+      <c r="O268" s="331"/>
       <c r="P268" s="10"/>
     </row>
     <row r="269" spans="1:16" ht="25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A269" s="9"/>
       <c r="B269" s="29"/>
       <c r="C269" s="30"/>
-      <c r="D269" s="339"/>
-      <c r="E269" s="340"/>
+      <c r="D269" s="332"/>
+      <c r="E269" s="333"/>
       <c r="F269" s="215"/>
       <c r="G269" s="215"/>
       <c r="H269" s="215"/>
       <c r="I269" s="31"/>
       <c r="J269" s="215"/>
       <c r="K269" s="215"/>
-      <c r="L269" s="341"/>
-      <c r="M269" s="341"/>
-      <c r="N269" s="341"/>
-      <c r="O269" s="342"/>
+      <c r="L269" s="334"/>
+      <c r="M269" s="334"/>
+      <c r="N269" s="334"/>
+      <c r="O269" s="335"/>
       <c r="P269" s="10"/>
     </row>
     <row r="270" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -28865,10 +28901,10 @@
       <c r="C274" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="D274" s="328" t="s">
+      <c r="D274" s="336" t="s">
         <v>30</v>
       </c>
-      <c r="E274" s="329"/>
+      <c r="E274" s="337"/>
       <c r="F274" s="25" t="s">
         <v>31</v>
       </c>
@@ -28887,12 +28923,12 @@
       <c r="K274" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="L274" s="330" t="s">
+      <c r="L274" s="338" t="s">
         <v>37</v>
       </c>
-      <c r="M274" s="330"/>
-      <c r="N274" s="330"/>
-      <c r="O274" s="331"/>
+      <c r="M274" s="338"/>
+      <c r="N274" s="338"/>
+      <c r="O274" s="339"/>
       <c r="P274" s="10"/>
     </row>
     <row r="275" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -28903,10 +28939,10 @@
       <c r="C275" s="27" t="s">
         <v>383</v>
       </c>
-      <c r="D275" s="332" t="s">
+      <c r="D275" s="328" t="s">
         <v>386</v>
       </c>
-      <c r="E275" s="333"/>
+      <c r="E275" s="329"/>
       <c r="F275" s="214"/>
       <c r="G275" s="214"/>
       <c r="H275" s="214" t="s">
@@ -28917,12 +28953,12 @@
       </c>
       <c r="J275" s="214"/>
       <c r="K275" s="214"/>
-      <c r="L275" s="334" t="s">
+      <c r="L275" s="330" t="s">
         <v>387</v>
       </c>
-      <c r="M275" s="334"/>
-      <c r="N275" s="334"/>
-      <c r="O275" s="335"/>
+      <c r="M275" s="330"/>
+      <c r="N275" s="330"/>
+      <c r="O275" s="331"/>
       <c r="P275" s="10"/>
     </row>
     <row r="276" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -28933,10 +28969,10 @@
       <c r="C276" s="27" t="s">
         <v>380</v>
       </c>
-      <c r="D276" s="332" t="s">
+      <c r="D276" s="328" t="s">
         <v>388</v>
       </c>
-      <c r="E276" s="333"/>
+      <c r="E276" s="329"/>
       <c r="F276" s="214"/>
       <c r="G276" s="214"/>
       <c r="H276" s="214" t="s">
@@ -28949,10 +28985,10 @@
         <v>255</v>
       </c>
       <c r="K276" s="214"/>
-      <c r="L276" s="334"/>
-      <c r="M276" s="334"/>
-      <c r="N276" s="334"/>
-      <c r="O276" s="335"/>
+      <c r="L276" s="330"/>
+      <c r="M276" s="330"/>
+      <c r="N276" s="330"/>
+      <c r="O276" s="331"/>
       <c r="P276" s="10"/>
     </row>
     <row r="277" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -28977,10 +29013,10 @@
         <v>255</v>
       </c>
       <c r="K277" s="214"/>
-      <c r="L277" s="334"/>
-      <c r="M277" s="334"/>
-      <c r="N277" s="334"/>
-      <c r="O277" s="335"/>
+      <c r="L277" s="330"/>
+      <c r="M277" s="330"/>
+      <c r="N277" s="330"/>
+      <c r="O277" s="331"/>
       <c r="P277" s="10"/>
     </row>
     <row r="278" spans="1:16" ht="25" thickBot="1" x14ac:dyDescent="0.35">
@@ -29005,12 +29041,12 @@
       </c>
       <c r="J278" s="215"/>
       <c r="K278" s="215"/>
-      <c r="L278" s="341" t="s">
+      <c r="L278" s="334" t="s">
         <v>416</v>
       </c>
-      <c r="M278" s="341"/>
-      <c r="N278" s="341"/>
-      <c r="O278" s="342"/>
+      <c r="M278" s="334"/>
+      <c r="N278" s="334"/>
+      <c r="O278" s="335"/>
       <c r="P278" s="10"/>
     </row>
     <row r="279" spans="1:16" x14ac:dyDescent="0.2">
@@ -29097,10 +29133,10 @@
       <c r="C283" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="D283" s="328" t="s">
+      <c r="D283" s="336" t="s">
         <v>30</v>
       </c>
-      <c r="E283" s="329"/>
+      <c r="E283" s="337"/>
       <c r="F283" s="25" t="s">
         <v>31</v>
       </c>
@@ -29119,12 +29155,12 @@
       <c r="K283" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="L283" s="330" t="s">
+      <c r="L283" s="338" t="s">
         <v>37</v>
       </c>
-      <c r="M283" s="330"/>
-      <c r="N283" s="330"/>
-      <c r="O283" s="331"/>
+      <c r="M283" s="338"/>
+      <c r="N283" s="338"/>
+      <c r="O283" s="339"/>
       <c r="P283" s="10"/>
     </row>
     <row r="284" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -29135,10 +29171,10 @@
       <c r="C284" s="27" t="s">
         <v>393</v>
       </c>
-      <c r="D284" s="332" t="s">
+      <c r="D284" s="328" t="s">
         <v>403</v>
       </c>
-      <c r="E284" s="333"/>
+      <c r="E284" s="329"/>
       <c r="F284" s="214"/>
       <c r="G284" s="214"/>
       <c r="H284" s="214" t="s">
@@ -29151,10 +29187,10 @@
         <v>255</v>
       </c>
       <c r="K284" s="214"/>
-      <c r="L284" s="334"/>
-      <c r="M284" s="334"/>
-      <c r="N284" s="334"/>
-      <c r="O284" s="335"/>
+      <c r="L284" s="330"/>
+      <c r="M284" s="330"/>
+      <c r="N284" s="330"/>
+      <c r="O284" s="331"/>
       <c r="P284" s="10"/>
     </row>
     <row r="285" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -29165,10 +29201,10 @@
       <c r="C285" s="27" t="s">
         <v>394</v>
       </c>
-      <c r="D285" s="332" t="s">
+      <c r="D285" s="328" t="s">
         <v>396</v>
       </c>
-      <c r="E285" s="333"/>
+      <c r="E285" s="329"/>
       <c r="F285" s="214"/>
       <c r="G285" s="214"/>
       <c r="H285" s="214" t="s">
@@ -29181,12 +29217,12 @@
         <v>255</v>
       </c>
       <c r="K285" s="214"/>
-      <c r="L285" s="334" t="s">
+      <c r="L285" s="330" t="s">
         <v>395</v>
       </c>
-      <c r="M285" s="334"/>
-      <c r="N285" s="334"/>
-      <c r="O285" s="335"/>
+      <c r="M285" s="330"/>
+      <c r="N285" s="330"/>
+      <c r="O285" s="331"/>
       <c r="P285" s="10"/>
     </row>
     <row r="286" spans="1:16" ht="24" x14ac:dyDescent="0.2">
@@ -29197,10 +29233,10 @@
       <c r="C286" s="28" t="s">
         <v>397</v>
       </c>
-      <c r="D286" s="343" t="s">
+      <c r="D286" s="340" t="s">
         <v>402</v>
       </c>
-      <c r="E286" s="344"/>
+      <c r="E286" s="341"/>
       <c r="F286" s="214"/>
       <c r="G286" s="214"/>
       <c r="H286" s="214" t="s">
@@ -29213,10 +29249,10 @@
         <v>255</v>
       </c>
       <c r="K286" s="214"/>
-      <c r="L286" s="345"/>
-      <c r="M286" s="334"/>
-      <c r="N286" s="334"/>
-      <c r="O286" s="335"/>
+      <c r="L286" s="342"/>
+      <c r="M286" s="330"/>
+      <c r="N286" s="330"/>
+      <c r="O286" s="331"/>
       <c r="P286" s="10"/>
     </row>
     <row r="287" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -29227,10 +29263,10 @@
       <c r="C287" s="27" t="s">
         <v>398</v>
       </c>
-      <c r="D287" s="332" t="s">
+      <c r="D287" s="328" t="s">
         <v>401</v>
       </c>
-      <c r="E287" s="333"/>
+      <c r="E287" s="329"/>
       <c r="F287" s="214"/>
       <c r="G287" s="214"/>
       <c r="H287" s="214" t="s">
@@ -29241,12 +29277,12 @@
       </c>
       <c r="J287" s="214"/>
       <c r="K287" s="214"/>
-      <c r="L287" s="334" t="s">
+      <c r="L287" s="330" t="s">
         <v>254</v>
       </c>
-      <c r="M287" s="334"/>
-      <c r="N287" s="334"/>
-      <c r="O287" s="335"/>
+      <c r="M287" s="330"/>
+      <c r="N287" s="330"/>
+      <c r="O287" s="331"/>
       <c r="P287" s="10"/>
     </row>
     <row r="288" spans="1:16" ht="24" x14ac:dyDescent="0.3">
@@ -29257,10 +29293,10 @@
       <c r="C288" s="27" t="s">
         <v>399</v>
       </c>
-      <c r="D288" s="332" t="s">
+      <c r="D288" s="328" t="s">
         <v>400</v>
       </c>
-      <c r="E288" s="333"/>
+      <c r="E288" s="329"/>
       <c r="F288" s="214"/>
       <c r="G288" s="214"/>
       <c r="H288" s="214"/>
@@ -29271,30 +29307,30 @@
       <c r="K288" s="214" t="s">
         <v>191</v>
       </c>
-      <c r="L288" s="334" t="s">
+      <c r="L288" s="330" t="s">
         <v>270</v>
       </c>
-      <c r="M288" s="334"/>
-      <c r="N288" s="334"/>
-      <c r="O288" s="335"/>
+      <c r="M288" s="330"/>
+      <c r="N288" s="330"/>
+      <c r="O288" s="331"/>
       <c r="P288" s="10"/>
     </row>
     <row r="289" spans="1:16" ht="25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A289" s="9"/>
       <c r="B289" s="29"/>
       <c r="C289" s="30"/>
-      <c r="D289" s="339"/>
-      <c r="E289" s="340"/>
+      <c r="D289" s="332"/>
+      <c r="E289" s="333"/>
       <c r="F289" s="215"/>
       <c r="G289" s="215"/>
       <c r="H289" s="215"/>
       <c r="I289" s="31"/>
       <c r="J289" s="215"/>
       <c r="K289" s="215"/>
-      <c r="L289" s="341"/>
-      <c r="M289" s="341"/>
-      <c r="N289" s="341"/>
-      <c r="O289" s="342"/>
+      <c r="L289" s="334"/>
+      <c r="M289" s="334"/>
+      <c r="N289" s="334"/>
+      <c r="O289" s="335"/>
       <c r="P289" s="10"/>
     </row>
     <row r="290" spans="1:16" x14ac:dyDescent="0.2">
@@ -29351,8 +29387,568 @@
       <c r="O292" s="12"/>
       <c r="P292" s="13"/>
     </row>
+    <row r="293" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="294" spans="1:16" ht="25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A294" s="9"/>
+      <c r="B294" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="C294" s="3"/>
+      <c r="D294" s="231" t="s">
+        <v>418</v>
+      </c>
+      <c r="E294" s="33"/>
+      <c r="F294" s="33"/>
+      <c r="G294" s="33"/>
+      <c r="H294" s="34"/>
+      <c r="I294" s="3"/>
+      <c r="J294" s="3"/>
+      <c r="K294" s="3"/>
+      <c r="L294" s="3"/>
+      <c r="M294" s="3"/>
+      <c r="N294" s="3"/>
+      <c r="O294" s="44"/>
+      <c r="P294" s="10"/>
+    </row>
+    <row r="295" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A295" s="9"/>
+      <c r="B295" s="3"/>
+      <c r="C295" s="3"/>
+      <c r="D295" s="3"/>
+      <c r="E295" s="3"/>
+      <c r="F295" s="3"/>
+      <c r="G295" s="3"/>
+      <c r="H295" s="3"/>
+      <c r="I295" s="3"/>
+      <c r="J295" s="3"/>
+      <c r="K295" s="3"/>
+      <c r="L295" s="3"/>
+      <c r="M295" s="3"/>
+      <c r="N295" s="3"/>
+      <c r="O295" s="3"/>
+      <c r="P295" s="10"/>
+    </row>
+    <row r="296" spans="1:16" ht="24" x14ac:dyDescent="0.3">
+      <c r="A296" s="9"/>
+      <c r="B296" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C296" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="D296" s="336" t="s">
+        <v>30</v>
+      </c>
+      <c r="E296" s="337"/>
+      <c r="F296" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="G296" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="H296" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="I296" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="J296" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="K296" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="L296" s="338" t="s">
+        <v>37</v>
+      </c>
+      <c r="M296" s="338"/>
+      <c r="N296" s="338"/>
+      <c r="O296" s="339"/>
+      <c r="P296" s="10"/>
+    </row>
+    <row r="297" spans="1:16" ht="24" x14ac:dyDescent="0.3">
+      <c r="A297" s="9"/>
+      <c r="B297" s="26">
+        <v>1</v>
+      </c>
+      <c r="C297" s="27" t="s">
+        <v>419</v>
+      </c>
+      <c r="D297" s="328"/>
+      <c r="E297" s="329"/>
+      <c r="F297" s="214"/>
+      <c r="G297" s="214"/>
+      <c r="H297" s="214" t="s">
+        <v>191</v>
+      </c>
+      <c r="I297" s="28" t="s">
+        <v>190</v>
+      </c>
+      <c r="J297" s="214">
+        <v>255</v>
+      </c>
+      <c r="K297" s="214"/>
+      <c r="L297" s="330"/>
+      <c r="M297" s="330"/>
+      <c r="N297" s="330"/>
+      <c r="O297" s="331"/>
+      <c r="P297" s="10"/>
+    </row>
+    <row r="298" spans="1:16" ht="24" x14ac:dyDescent="0.3">
+      <c r="A298" s="9"/>
+      <c r="B298" s="26">
+        <v>2</v>
+      </c>
+      <c r="C298" s="27" t="s">
+        <v>420</v>
+      </c>
+      <c r="D298" s="328"/>
+      <c r="E298" s="329"/>
+      <c r="F298" s="214"/>
+      <c r="G298" s="214"/>
+      <c r="H298" s="214" t="s">
+        <v>191</v>
+      </c>
+      <c r="I298" s="28" t="s">
+        <v>188</v>
+      </c>
+      <c r="J298" s="214"/>
+      <c r="K298" s="214"/>
+      <c r="L298" s="330" t="s">
+        <v>354</v>
+      </c>
+      <c r="M298" s="330"/>
+      <c r="N298" s="330"/>
+      <c r="O298" s="331"/>
+      <c r="P298" s="10"/>
+    </row>
+    <row r="299" spans="1:16" ht="24" x14ac:dyDescent="0.2">
+      <c r="A299" s="9"/>
+      <c r="B299" s="234">
+        <v>3</v>
+      </c>
+      <c r="C299" s="28" t="s">
+        <v>421</v>
+      </c>
+      <c r="D299" s="340"/>
+      <c r="E299" s="341"/>
+      <c r="F299" s="214"/>
+      <c r="G299" s="214"/>
+      <c r="H299" s="214" t="s">
+        <v>191</v>
+      </c>
+      <c r="I299" s="28" t="s">
+        <v>188</v>
+      </c>
+      <c r="J299" s="214"/>
+      <c r="K299" s="214"/>
+      <c r="L299" s="342" t="s">
+        <v>350</v>
+      </c>
+      <c r="M299" s="330"/>
+      <c r="N299" s="330"/>
+      <c r="O299" s="331"/>
+      <c r="P299" s="10"/>
+    </row>
+    <row r="300" spans="1:16" ht="24" x14ac:dyDescent="0.3">
+      <c r="A300" s="9"/>
+      <c r="B300" s="26">
+        <v>4</v>
+      </c>
+      <c r="C300" s="27" t="s">
+        <v>405</v>
+      </c>
+      <c r="D300" s="328"/>
+      <c r="E300" s="329"/>
+      <c r="F300" s="214"/>
+      <c r="G300" s="214"/>
+      <c r="H300" s="214" t="s">
+        <v>191</v>
+      </c>
+      <c r="I300" s="28" t="s">
+        <v>188</v>
+      </c>
+      <c r="J300" s="214"/>
+      <c r="K300" s="214"/>
+      <c r="L300" s="330"/>
+      <c r="M300" s="330"/>
+      <c r="N300" s="330"/>
+      <c r="O300" s="331"/>
+      <c r="P300" s="10"/>
+    </row>
+    <row r="301" spans="1:16" ht="24" x14ac:dyDescent="0.3">
+      <c r="A301" s="9"/>
+      <c r="B301" s="26">
+        <v>5</v>
+      </c>
+      <c r="C301" s="27" t="s">
+        <v>335</v>
+      </c>
+      <c r="D301" s="328"/>
+      <c r="E301" s="329"/>
+      <c r="F301" s="214"/>
+      <c r="G301" s="214"/>
+      <c r="H301" s="214" t="s">
+        <v>191</v>
+      </c>
+      <c r="I301" s="28" t="s">
+        <v>188</v>
+      </c>
+      <c r="J301" s="214"/>
+      <c r="K301" s="214"/>
+      <c r="L301" s="330"/>
+      <c r="M301" s="330"/>
+      <c r="N301" s="330"/>
+      <c r="O301" s="331"/>
+      <c r="P301" s="10"/>
+    </row>
+    <row r="302" spans="1:16" ht="24" x14ac:dyDescent="0.3">
+      <c r="A302" s="9"/>
+      <c r="B302" s="26">
+        <v>6</v>
+      </c>
+      <c r="C302" s="27" t="s">
+        <v>422</v>
+      </c>
+      <c r="D302" s="328"/>
+      <c r="E302" s="329"/>
+      <c r="F302" s="214"/>
+      <c r="G302" s="214"/>
+      <c r="H302" s="214" t="s">
+        <v>191</v>
+      </c>
+      <c r="I302" s="28" t="s">
+        <v>190</v>
+      </c>
+      <c r="J302" s="214">
+        <v>255</v>
+      </c>
+      <c r="K302" s="214"/>
+      <c r="L302" s="330"/>
+      <c r="M302" s="330"/>
+      <c r="N302" s="330"/>
+      <c r="O302" s="331"/>
+      <c r="P302" s="10"/>
+    </row>
+    <row r="303" spans="1:16" ht="24" x14ac:dyDescent="0.3">
+      <c r="A303" s="9"/>
+      <c r="B303" s="26">
+        <v>7</v>
+      </c>
+      <c r="C303" s="27" t="s">
+        <v>423</v>
+      </c>
+      <c r="D303" s="328"/>
+      <c r="E303" s="329"/>
+      <c r="F303" s="214"/>
+      <c r="G303" s="214"/>
+      <c r="H303" s="214" t="s">
+        <v>191</v>
+      </c>
+      <c r="I303" s="28" t="s">
+        <v>188</v>
+      </c>
+      <c r="J303" s="214"/>
+      <c r="K303" s="214"/>
+      <c r="L303" s="330" t="s">
+        <v>424</v>
+      </c>
+      <c r="M303" s="330"/>
+      <c r="N303" s="330"/>
+      <c r="O303" s="331"/>
+      <c r="P303" s="10"/>
+    </row>
+    <row r="304" spans="1:16" ht="25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A304" s="9"/>
+      <c r="B304" s="29"/>
+      <c r="C304" s="30"/>
+      <c r="D304" s="332"/>
+      <c r="E304" s="333"/>
+      <c r="F304" s="215"/>
+      <c r="G304" s="215"/>
+      <c r="H304" s="215"/>
+      <c r="I304" s="31"/>
+      <c r="J304" s="215"/>
+      <c r="K304" s="215"/>
+      <c r="L304" s="334"/>
+      <c r="M304" s="334"/>
+      <c r="N304" s="334"/>
+      <c r="O304" s="335"/>
+      <c r="P304" s="10"/>
+    </row>
+    <row r="306" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="307" spans="1:16" ht="25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A307" s="9"/>
+      <c r="B307" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="C307" s="3"/>
+      <c r="D307" s="231" t="s">
+        <v>425</v>
+      </c>
+      <c r="E307" s="33"/>
+      <c r="F307" s="33"/>
+      <c r="G307" s="33"/>
+      <c r="H307" s="34"/>
+      <c r="I307" s="3"/>
+      <c r="J307" s="3"/>
+      <c r="K307" s="3"/>
+      <c r="L307" s="3"/>
+      <c r="M307" s="3"/>
+      <c r="N307" s="3"/>
+      <c r="O307" s="44"/>
+      <c r="P307" s="10"/>
+    </row>
+    <row r="308" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A308" s="9"/>
+      <c r="B308" s="3"/>
+      <c r="C308" s="3"/>
+      <c r="D308" s="3"/>
+      <c r="E308" s="3"/>
+      <c r="F308" s="3"/>
+      <c r="G308" s="3"/>
+      <c r="H308" s="3"/>
+      <c r="I308" s="3"/>
+      <c r="J308" s="3"/>
+      <c r="K308" s="3"/>
+      <c r="L308" s="3"/>
+      <c r="M308" s="3"/>
+      <c r="N308" s="3"/>
+      <c r="O308" s="3"/>
+      <c r="P308" s="10"/>
+    </row>
+    <row r="309" spans="1:16" ht="24" x14ac:dyDescent="0.3">
+      <c r="A309" s="9"/>
+      <c r="B309" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C309" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="D309" s="336" t="s">
+        <v>30</v>
+      </c>
+      <c r="E309" s="337"/>
+      <c r="F309" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="G309" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="H309" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="I309" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="J309" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="K309" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="L309" s="338" t="s">
+        <v>37</v>
+      </c>
+      <c r="M309" s="338"/>
+      <c r="N309" s="338"/>
+      <c r="O309" s="339"/>
+      <c r="P309" s="10"/>
+    </row>
+    <row r="310" spans="1:16" ht="24" x14ac:dyDescent="0.3">
+      <c r="A310" s="9"/>
+      <c r="B310" s="26">
+        <v>1</v>
+      </c>
+      <c r="C310" s="27" t="s">
+        <v>237</v>
+      </c>
+      <c r="D310" s="328"/>
+      <c r="E310" s="329"/>
+      <c r="F310" s="214"/>
+      <c r="G310" s="214"/>
+      <c r="H310" s="214" t="s">
+        <v>191</v>
+      </c>
+      <c r="I310" s="28" t="s">
+        <v>188</v>
+      </c>
+      <c r="J310" s="214"/>
+      <c r="K310" s="214" t="s">
+        <v>191</v>
+      </c>
+      <c r="L310" s="330" t="s">
+        <v>426</v>
+      </c>
+      <c r="M310" s="330"/>
+      <c r="N310" s="330"/>
+      <c r="O310" s="331"/>
+      <c r="P310" s="10"/>
+    </row>
+    <row r="311" spans="1:16" ht="24" x14ac:dyDescent="0.3">
+      <c r="A311" s="9"/>
+      <c r="B311" s="26">
+        <v>2</v>
+      </c>
+      <c r="C311" s="27" t="s">
+        <v>314</v>
+      </c>
+      <c r="D311" s="328"/>
+      <c r="E311" s="329"/>
+      <c r="F311" s="214"/>
+      <c r="G311" s="214"/>
+      <c r="H311" s="214" t="s">
+        <v>191</v>
+      </c>
+      <c r="I311" s="28" t="s">
+        <v>188</v>
+      </c>
+      <c r="J311" s="214"/>
+      <c r="K311" s="214"/>
+      <c r="L311" s="330"/>
+      <c r="M311" s="330"/>
+      <c r="N311" s="330"/>
+      <c r="O311" s="331"/>
+      <c r="P311" s="10"/>
+    </row>
+    <row r="312" spans="1:16" ht="24" x14ac:dyDescent="0.2">
+      <c r="A312" s="9"/>
+      <c r="B312" s="234">
+        <v>3</v>
+      </c>
+      <c r="C312" s="28" t="s">
+        <v>428</v>
+      </c>
+      <c r="D312" s="340"/>
+      <c r="E312" s="341"/>
+      <c r="F312" s="214"/>
+      <c r="G312" s="214"/>
+      <c r="H312" s="214" t="s">
+        <v>191</v>
+      </c>
+      <c r="I312" s="28" t="s">
+        <v>190</v>
+      </c>
+      <c r="J312" s="214">
+        <v>20</v>
+      </c>
+      <c r="K312" s="214"/>
+      <c r="L312" s="342"/>
+      <c r="M312" s="330"/>
+      <c r="N312" s="330"/>
+      <c r="O312" s="331"/>
+      <c r="P312" s="10"/>
+    </row>
+    <row r="313" spans="1:16" ht="24" x14ac:dyDescent="0.3">
+      <c r="A313" s="9"/>
+      <c r="B313" s="26">
+        <v>4</v>
+      </c>
+      <c r="C313" s="27" t="s">
+        <v>427</v>
+      </c>
+      <c r="D313" s="328"/>
+      <c r="E313" s="329"/>
+      <c r="F313" s="214"/>
+      <c r="G313" s="214"/>
+      <c r="H313" s="214" t="s">
+        <v>191</v>
+      </c>
+      <c r="I313" s="28" t="s">
+        <v>188</v>
+      </c>
+      <c r="J313" s="214"/>
+      <c r="K313" s="214"/>
+      <c r="L313" s="330"/>
+      <c r="M313" s="330"/>
+      <c r="N313" s="330"/>
+      <c r="O313" s="331"/>
+      <c r="P313" s="10"/>
+    </row>
+    <row r="314" spans="1:16" ht="24" x14ac:dyDescent="0.3">
+      <c r="A314" s="9"/>
+      <c r="B314" s="26">
+        <v>5</v>
+      </c>
+      <c r="C314" s="27" t="s">
+        <v>429</v>
+      </c>
+      <c r="D314" s="328"/>
+      <c r="E314" s="329"/>
+      <c r="F314" s="214"/>
+      <c r="G314" s="214"/>
+      <c r="H314" s="214" t="s">
+        <v>191</v>
+      </c>
+      <c r="I314" s="28" t="s">
+        <v>190</v>
+      </c>
+      <c r="J314" s="214">
+        <v>20</v>
+      </c>
+      <c r="K314" s="214"/>
+      <c r="L314" s="330"/>
+      <c r="M314" s="330"/>
+      <c r="N314" s="330"/>
+      <c r="O314" s="331"/>
+      <c r="P314" s="10"/>
+    </row>
+    <row r="315" spans="1:16" ht="24" x14ac:dyDescent="0.3">
+      <c r="A315" s="9"/>
+      <c r="B315" s="26"/>
+      <c r="C315" s="27"/>
+      <c r="D315" s="328"/>
+      <c r="E315" s="329"/>
+      <c r="F315" s="214"/>
+      <c r="G315" s="214"/>
+      <c r="H315" s="214"/>
+      <c r="I315" s="28"/>
+      <c r="J315" s="214"/>
+      <c r="K315" s="214"/>
+      <c r="L315" s="330"/>
+      <c r="M315" s="330"/>
+      <c r="N315" s="330"/>
+      <c r="O315" s="331"/>
+      <c r="P315" s="10"/>
+    </row>
+    <row r="316" spans="1:16" ht="24" x14ac:dyDescent="0.3">
+      <c r="A316" s="9"/>
+      <c r="B316" s="26"/>
+      <c r="C316" s="27"/>
+      <c r="D316" s="328"/>
+      <c r="E316" s="329"/>
+      <c r="F316" s="214"/>
+      <c r="G316" s="214"/>
+      <c r="H316" s="214"/>
+      <c r="I316" s="28"/>
+      <c r="J316" s="214"/>
+      <c r="K316" s="214"/>
+      <c r="L316" s="330"/>
+      <c r="M316" s="330"/>
+      <c r="N316" s="330"/>
+      <c r="O316" s="331"/>
+      <c r="P316" s="10"/>
+    </row>
+    <row r="317" spans="1:16" ht="25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A317" s="9"/>
+      <c r="B317" s="29"/>
+      <c r="C317" s="30"/>
+      <c r="D317" s="332"/>
+      <c r="E317" s="333"/>
+      <c r="F317" s="215"/>
+      <c r="G317" s="215"/>
+      <c r="H317" s="215"/>
+      <c r="I317" s="31"/>
+      <c r="J317" s="215"/>
+      <c r="K317" s="215"/>
+      <c r="L317" s="334"/>
+      <c r="M317" s="334"/>
+      <c r="N317" s="334"/>
+      <c r="O317" s="335"/>
+      <c r="P317" s="10"/>
+    </row>
   </sheetData>
-  <mergeCells count="321">
+  <mergeCells count="357">
     <mergeCell ref="L122:O122"/>
     <mergeCell ref="L123:O123"/>
     <mergeCell ref="D127:E127"/>
@@ -29674,6 +30270,42 @@
     <mergeCell ref="L106:O106"/>
     <mergeCell ref="D107:E107"/>
     <mergeCell ref="L107:O107"/>
+    <mergeCell ref="D301:E301"/>
+    <mergeCell ref="L301:O301"/>
+    <mergeCell ref="D304:E304"/>
+    <mergeCell ref="L304:O304"/>
+    <mergeCell ref="D302:E302"/>
+    <mergeCell ref="L302:O302"/>
+    <mergeCell ref="D303:E303"/>
+    <mergeCell ref="L303:O303"/>
+    <mergeCell ref="D296:E296"/>
+    <mergeCell ref="L296:O296"/>
+    <mergeCell ref="D297:E297"/>
+    <mergeCell ref="L297:O297"/>
+    <mergeCell ref="D298:E298"/>
+    <mergeCell ref="L298:O298"/>
+    <mergeCell ref="D299:E299"/>
+    <mergeCell ref="L299:O299"/>
+    <mergeCell ref="D300:E300"/>
+    <mergeCell ref="L300:O300"/>
+    <mergeCell ref="D314:E314"/>
+    <mergeCell ref="L314:O314"/>
+    <mergeCell ref="D315:E315"/>
+    <mergeCell ref="L315:O315"/>
+    <mergeCell ref="D316:E316"/>
+    <mergeCell ref="L316:O316"/>
+    <mergeCell ref="D317:E317"/>
+    <mergeCell ref="L317:O317"/>
+    <mergeCell ref="D309:E309"/>
+    <mergeCell ref="L309:O309"/>
+    <mergeCell ref="D310:E310"/>
+    <mergeCell ref="L310:O310"/>
+    <mergeCell ref="D311:E311"/>
+    <mergeCell ref="L311:O311"/>
+    <mergeCell ref="D312:E312"/>
+    <mergeCell ref="L312:O312"/>
+    <mergeCell ref="D313:E313"/>
+    <mergeCell ref="L313:O313"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -29748,7 +30380,7 @@
       </c>
       <c r="P2" s="280">
         <f ca="1">NOW()</f>
-        <v>44573.893278587966</v>
+        <v>44573.955704398148</v>
       </c>
       <c r="Q2" s="281"/>
     </row>
@@ -30678,8 +31310,8 @@
   </sheetPr>
   <dimension ref="A1:Q106"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="140" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection sqref="A1:B2"/>
+    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A2" zoomScaleNormal="140" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -30743,7 +31375,7 @@
       </c>
       <c r="N2" s="280">
         <f ca="1">NOW()</f>
-        <v>44573.893278587966</v>
+        <v>44573.955704398148</v>
       </c>
       <c r="O2" s="281"/>
       <c r="P2" s="61"/>
@@ -32024,7 +32656,7 @@
       </c>
       <c r="AK2" s="280">
         <f ca="1">NOW()</f>
-        <v>44573.893278587966</v>
+        <v>44573.955704398148</v>
       </c>
       <c r="AL2" s="281"/>
       <c r="AM2" s="61"/>
@@ -32541,7 +33173,7 @@
       </c>
       <c r="T2" s="280">
         <f ca="1">NOW()</f>
-        <v>44573.893278587966</v>
+        <v>44573.955704398148</v>
       </c>
       <c r="U2" s="281"/>
     </row>
@@ -33954,7 +34586,7 @@
       </c>
       <c r="P2" s="280">
         <f ca="1">NOW()</f>
-        <v>44573.893278587966</v>
+        <v>44573.955704398148</v>
       </c>
       <c r="Q2" s="281"/>
     </row>
@@ -39557,7 +40189,7 @@
       </c>
       <c r="S2" s="280">
         <f ca="1">NOW()</f>
-        <v>44573.893278587966</v>
+        <v>44573.955704398148</v>
       </c>
       <c r="T2" s="281"/>
     </row>
@@ -46332,7 +46964,7 @@
       </c>
       <c r="T2" s="280">
         <f ca="1">NOW()</f>
-        <v>44573.893278587966</v>
+        <v>44573.955704398148</v>
       </c>
       <c r="U2" s="281"/>
     </row>
@@ -48582,7 +49214,7 @@
       </c>
       <c r="P2" s="280">
         <f ca="1">NOW()</f>
-        <v>44573.893278587966</v>
+        <v>44573.955704398148</v>
       </c>
       <c r="Q2" s="281"/>
     </row>

</xml_diff>